<commit_message>
Start Statistical Model section
</commit_message>
<xml_diff>
--- a/Descr.xlsx
+++ b/Descr.xlsx
@@ -8,25 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FSAN\Adm_Yield\Manuscript\Timing-in-Admission-Yield\Timing-in-Admission-Yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB69303D-BFE0-4DFA-AA69-B875D896B1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C64756-EB87-4B9B-A14C-7F15A10DDFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Table 4" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>Period</t>
   </si>
@@ -55,18 +68,9 @@
     <t>Variable Name</t>
   </si>
   <si>
-    <t>Inst FinAid</t>
-  </si>
-  <si>
-    <t>Institutional grants offered</t>
-  </si>
-  <si>
     <t>Loan</t>
   </si>
   <si>
-    <t>Loan borrowed</t>
-  </si>
-  <si>
     <t>Pell</t>
   </si>
   <si>
@@ -121,9 +125,6 @@
     <t>EFC</t>
   </si>
   <si>
-    <t>Expected family contribution</t>
-  </si>
-  <si>
     <t>HS GPA</t>
   </si>
   <si>
@@ -203,13 +204,63 @@
   </si>
   <si>
     <t>1 - Februrary</t>
+  </si>
+  <si>
+    <t>Institutional Grant</t>
+  </si>
+  <si>
+    <t>Institutional grants offered over COA</t>
+  </si>
+  <si>
+    <t>Loan borrowed over COA</t>
+  </si>
+  <si>
+    <t>Expected family contribution over COA</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>Mean/Pct</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>S.D.</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,18 +286,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -526,52 +583,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" activeCellId="2" sqref="C3:C10 E3:E10 G3:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>2020</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2">
         <v>2021</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2">
         <v>2022</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>58</v>
+      <c r="A3" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B3">
         <v>15866</v>
@@ -593,8 +650,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>51</v>
+      <c r="A4" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B4">
         <v>16457</v>
@@ -616,8 +673,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>52</v>
+      <c r="A5" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B5">
         <v>16673</v>
@@ -639,8 +696,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>53</v>
+      <c r="A6" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B6">
         <v>16385</v>
@@ -662,8 +719,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>54</v>
+      <c r="A7" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B7">
         <v>16112</v>
@@ -685,8 +742,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>55</v>
+      <c r="A8" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B8">
         <v>15779</v>
@@ -708,8 +765,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>56</v>
+      <c r="A9" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B9">
         <v>15739</v>
@@ -731,8 +788,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>57</v>
+      <c r="A10" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B10">
         <v>15129</v>
@@ -769,13 +826,13 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D20"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -790,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -809,206 +866,1187 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E612A584-0A1D-4752-B9BA-51A64B61275A}">
+  <dimension ref="A1:G44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.1901057116</v>
+      </c>
+      <c r="D2">
+        <v>0.1245786413</v>
+      </c>
+      <c r="F2">
+        <v>0.83817508289999998</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.20064038949999999</v>
+      </c>
+      <c r="D3">
+        <v>0.12866403139999999</v>
+      </c>
+      <c r="F3">
+        <v>0.95765789379999999</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.2029414182</v>
+      </c>
+      <c r="D4">
+        <v>0.13228007059999999</v>
+      </c>
+      <c r="F4">
+        <v>0.99757113750000004</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.2012305532</v>
+      </c>
+      <c r="D5">
+        <v>0.13388997180000001</v>
+      </c>
+      <c r="F5">
+        <v>1.0872164814</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.20199927919999999</v>
+      </c>
+      <c r="D6">
+        <v>0.13409681509999999</v>
+      </c>
+      <c r="F6">
+        <v>1.0872164814</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.2046729293</v>
+      </c>
+      <c r="D7">
+        <v>0.13269538340000001</v>
+      </c>
+      <c r="F7">
+        <v>1.0872164814</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.2037681268</v>
+      </c>
+      <c r="D8">
+        <v>0.13358940010000001</v>
+      </c>
+      <c r="F8">
+        <v>1.0872164814</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0.20496410970000001</v>
+      </c>
+      <c r="D9">
+        <v>0.13275757839999999</v>
+      </c>
+      <c r="F9">
+        <v>1.0872164814</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>7.0578047699999993E-2</v>
+      </c>
+      <c r="D10">
+        <v>4.9135036299999997E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.35744459610000001</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>7.89229704E-2</v>
+      </c>
+      <c r="D11">
+        <v>5.2576604899999997E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>8.1963344699999996E-2</v>
+      </c>
+      <c r="D12">
+        <v>5.16641906E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>8.1621849400000002E-2</v>
+      </c>
+      <c r="D13">
+        <v>5.15050144E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>8.2333335300000005E-2</v>
+      </c>
+      <c r="D14">
+        <v>5.1042771399999999E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>8.3052101599999997E-2</v>
+      </c>
+      <c r="D15">
+        <v>5.0326466600000001E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>8.2048893999999997E-2</v>
+      </c>
+      <c r="D16">
+        <v>5.04143752E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8.1723539600000006E-2</v>
+      </c>
+      <c r="D17">
+        <v>4.9808077399999998E-2</v>
+      </c>
+      <c r="F17">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.1197019547</v>
+      </c>
+      <c r="E18">
+        <v>6185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>4.9511424999999998E-2</v>
+      </c>
+      <c r="E19">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>4.2944563099999999E-2</v>
+      </c>
+      <c r="E20">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1.5829694299999999E-2</v>
+      </c>
+      <c r="E21">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>5.6730273000000003E-3</v>
+      </c>
+      <c r="E22">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>1.0739115E-3</v>
+      </c>
+      <c r="E23">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>9.2837687000000002E-3</v>
+      </c>
+      <c r="E24">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>5.4192930000000002E-4</v>
+      </c>
+      <c r="E25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.1901057116</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.1245786413</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.83817508289999998</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.20064038949999999</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0.12866403139999999</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.95765789379999999</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.2029414182</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.13228007059999999</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.99757113750000004</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.2012305532</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.13388997180000001</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1.0872164814</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.20199927919999999</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.13409681509999999</v>
+      </c>
+      <c r="E33" s="4">
+        <v>1.0872164814</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.2046729293</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.13269538340000001</v>
+      </c>
+      <c r="E34" s="4">
+        <v>1.0872164814</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.2037681268</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.13358940010000001</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1.0872164814</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.20496410970000001</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.13275757839999999</v>
+      </c>
+      <c r="E36" s="4">
+        <v>1.0872164814</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4">
+        <v>7.0578047699999993E-2</v>
+      </c>
+      <c r="D37" s="4">
+        <v>4.9135036299999997E-2</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0.35744459610000001</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" s="4">
+        <v>7.89229704E-2</v>
+      </c>
+      <c r="D38" s="4">
+        <v>5.2576604899999997E-2</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" s="4">
+        <v>8.1963344699999996E-2</v>
+      </c>
+      <c r="D39" s="4">
+        <v>5.16641906E-2</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" s="4">
+        <v>8.1621849400000002E-2</v>
+      </c>
+      <c r="D40" s="4">
+        <v>5.15050144E-2</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" s="4">
+        <v>8.2333335300000005E-2</v>
+      </c>
+      <c r="D41" s="4">
+        <v>5.1042771399999999E-2</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42" s="4">
+        <v>8.3052101599999997E-2</v>
+      </c>
+      <c r="D42" s="4">
+        <v>5.0326466600000001E-2</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43" s="4">
+        <v>8.2048893999999997E-2</v>
+      </c>
+      <c r="D43" s="4">
+        <v>5.04143752E-2</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44" s="4">
+        <v>8.1723539600000006E-2</v>
+      </c>
+      <c r="D44" s="4">
+        <v>4.9808077399999998E-2</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0.21121726129999999</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58FE35B-40E3-42B8-9716-51C7F560DCC8}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>10358</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.17724768129999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>7077</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.1211027071</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5">
+        <v>290.31270747999997</v>
+      </c>
+      <c r="D4" s="5">
+        <v>740.07746884000005</v>
+      </c>
+      <c r="E4" s="6">
+        <v>29531</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>2732</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4.6750402099999998E-2</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>3656</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6.2562031599999998E-2</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>5170</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8.8469831299999996E-2</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>42677</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.73029535580000005</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>1839</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3.1469249499999997E-2</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>20972</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.35887607379999997</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1.1906461261000001</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.6723132553</v>
+      </c>
+      <c r="E11" s="5">
+        <v>32.494930785999998</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5">
+        <v>3.7078460933000001</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.69971700299999995</v>
+      </c>
+      <c r="E12" s="5">
+        <v>4.25</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>7324</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.12532940889999999</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>3163</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5.41257401E-2</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>11809</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.20207741539999999</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>24059</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.41170129030000002</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="5">
+        <v>14.273092850999999</v>
+      </c>
+      <c r="D17" s="5">
+        <v>135.90821062000001</v>
+      </c>
+      <c r="E17" s="6">
+        <v>9945</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
interval of Parameter estimate Whether a varialbe has time-varying effect
</commit_message>
<xml_diff>
--- a/Descr.xlsx
+++ b/Descr.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FSAN\Adm_Yield\Manuscript\Timing-in-Admission-Yield\Timing-in-Admission-Yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C64756-EB87-4B9B-A14C-7F15A10DDFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7509FF84-8920-4845-8314-BA005FCBA6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7590" yWindow="6540" windowWidth="28800" windowHeight="10755" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
     <sheet name="Table 3" sheetId="4" r:id="rId3"/>
     <sheet name="Table 4" sheetId="3" r:id="rId4"/>
+    <sheet name="Table 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="244">
   <si>
     <t>Period</t>
   </si>
@@ -243,6 +244,534 @@
   </si>
   <si>
     <t>Mean</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Period 1</t>
+  </si>
+  <si>
+    <t>Period 2</t>
+  </si>
+  <si>
+    <t>Period 3</t>
+  </si>
+  <si>
+    <t>Period 4</t>
+  </si>
+  <si>
+    <t>Period 5</t>
+  </si>
+  <si>
+    <t>Period 6</t>
+  </si>
+  <si>
+    <t>Period 7</t>
+  </si>
+  <si>
+    <t>Period 8</t>
+  </si>
+  <si>
+    <t>(-7.76, -7.749)</t>
+  </si>
+  <si>
+    <t>(-8.969, -8.957)</t>
+  </si>
+  <si>
+    <t>(-8.001, -7.99)</t>
+  </si>
+  <si>
+    <t>(-7.777, -7.766)</t>
+  </si>
+  <si>
+    <t>(-7.305, -7.295)</t>
+  </si>
+  <si>
+    <t>(-7.7, -7.688)</t>
+  </si>
+  <si>
+    <t>(-6.593, -6.583)</t>
+  </si>
+  <si>
+    <t>(-6.071, -6.06)</t>
+  </si>
+  <si>
+    <t>(0.236, 0.259)</t>
+  </si>
+  <si>
+    <t>(1.095, 1.123)</t>
+  </si>
+  <si>
+    <t>(0.888, 0.916)</t>
+  </si>
+  <si>
+    <t>(1.212, 1.248)</t>
+  </si>
+  <si>
+    <t>(1.037, 1.072)</t>
+  </si>
+  <si>
+    <t>(1.333, 1.368)</t>
+  </si>
+  <si>
+    <t>(1.799, 1.822)</t>
+  </si>
+  <si>
+    <t>(1.081, 1.118)</t>
+  </si>
+  <si>
+    <t>(-0.086, -0.074)</t>
+  </si>
+  <si>
+    <t>(-0.346, -0.326)</t>
+  </si>
+  <si>
+    <t>(-0.057, -0.047)</t>
+  </si>
+  <si>
+    <t>(0.025, 0.034)</t>
+  </si>
+  <si>
+    <t>(-0.196, -0.182)</t>
+  </si>
+  <si>
+    <t>(-0.035, -0.026)</t>
+  </si>
+  <si>
+    <t>(-0.077, -0.069)</t>
+  </si>
+  <si>
+    <t>(-0.104, -0.095)</t>
+  </si>
+  <si>
+    <t>(-0.19, -0.17)</t>
+  </si>
+  <si>
+    <t>(-0.252, -0.231)</t>
+  </si>
+  <si>
+    <t>(-0.001, 0.015)</t>
+  </si>
+  <si>
+    <t>(0.194, 0.211)</t>
+  </si>
+  <si>
+    <t>(-0.101, -0.082)</t>
+  </si>
+  <si>
+    <t>(-0.164, -0.147)</t>
+  </si>
+  <si>
+    <t>(0.065, 0.079)</t>
+  </si>
+  <si>
+    <t>(0.002, 0.019)</t>
+  </si>
+  <si>
+    <t>(0.843, 0.864)</t>
+  </si>
+  <si>
+    <t>(0.88, 0.902)</t>
+  </si>
+  <si>
+    <t>(1.028, 1.047)</t>
+  </si>
+  <si>
+    <t>(0.974, 0.995)</t>
+  </si>
+  <si>
+    <t>(1.007, 1.028)</t>
+  </si>
+  <si>
+    <t>(1.128, 1.146)</t>
+  </si>
+  <si>
+    <t>(1.025, 1.042)</t>
+  </si>
+  <si>
+    <t>(1.101, 1.12)</t>
+  </si>
+  <si>
+    <t>(-0.356, -0.341)</t>
+  </si>
+  <si>
+    <t>(-0.057, -0.041)</t>
+  </si>
+  <si>
+    <t>(-0.308, -0.294)</t>
+  </si>
+  <si>
+    <t>(-0.202, -0.187)</t>
+  </si>
+  <si>
+    <t>(-0.054, -0.041)</t>
+  </si>
+  <si>
+    <t>(0.214, 0.226)</t>
+  </si>
+  <si>
+    <t>(0.069, 0.079)</t>
+  </si>
+  <si>
+    <t>(0.447, 0.458)</t>
+  </si>
+  <si>
+    <t>(-1.0, -0.965)</t>
+  </si>
+  <si>
+    <t>(-0.948, -0.913)</t>
+  </si>
+  <si>
+    <t>(-0.812, -0.779)</t>
+  </si>
+  <si>
+    <t>(-0.585, -0.552)</t>
+  </si>
+  <si>
+    <t>(-0.814, -0.779)</t>
+  </si>
+  <si>
+    <t>(-0.627, -0.594)</t>
+  </si>
+  <si>
+    <t>(-0.779, -0.748)</t>
+  </si>
+  <si>
+    <t>(-1.443, -1.373)</t>
+  </si>
+  <si>
+    <t>(-1.41, -1.342)</t>
+  </si>
+  <si>
+    <t>(-1.518, -1.449)</t>
+  </si>
+  <si>
+    <t>(-1.393, -1.323)</t>
+  </si>
+  <si>
+    <t>(-1.377, -1.308)</t>
+  </si>
+  <si>
+    <t>(-1.407, -1.339)</t>
+  </si>
+  <si>
+    <t>(-1.426, -1.358)</t>
+  </si>
+  <si>
+    <t>(-1.339, -1.272)</t>
+  </si>
+  <si>
+    <t>(-0.091, -0.084)</t>
+  </si>
+  <si>
+    <t>(-0.023, -0.017)</t>
+  </si>
+  <si>
+    <t>(0.027, 0.03)</t>
+  </si>
+  <si>
+    <t>(-0.046, -0.04)</t>
+  </si>
+  <si>
+    <t>(-0.094, -0.087)</t>
+  </si>
+  <si>
+    <t>(-0.026, -0.021)</t>
+  </si>
+  <si>
+    <t>(-0.063, -0.059)</t>
+  </si>
+  <si>
+    <t>(-0.052, -0.047)</t>
+  </si>
+  <si>
+    <t>(0.03, 0.052)</t>
+  </si>
+  <si>
+    <t>(0.11, 0.134)</t>
+  </si>
+  <si>
+    <t>(0.192, 0.211)</t>
+  </si>
+  <si>
+    <t>(0.05, 0.071)</t>
+  </si>
+  <si>
+    <t>(0.093, 0.112)</t>
+  </si>
+  <si>
+    <t>(0.103, 0.122)</t>
+  </si>
+  <si>
+    <t>(0.118, 0.134)</t>
+  </si>
+  <si>
+    <t>(0.499, 0.515)</t>
+  </si>
+  <si>
+    <t>(-0.486, -0.454)</t>
+  </si>
+  <si>
+    <t>(-0.456, -0.424)</t>
+  </si>
+  <si>
+    <t>(-0.537, -0.507)</t>
+  </si>
+  <si>
+    <t>(-0.315, -0.284)</t>
+  </si>
+  <si>
+    <t>(-0.531, -0.502)</t>
+  </si>
+  <si>
+    <t>(-0.458, -0.429)</t>
+  </si>
+  <si>
+    <t>(-0.572, -0.547)</t>
+  </si>
+  <si>
+    <t>(-0.418, -0.393)</t>
+  </si>
+  <si>
+    <t>(-0.329, -0.298)</t>
+  </si>
+  <si>
+    <t>(-0.342, -0.309)</t>
+  </si>
+  <si>
+    <t>(-0.412, -0.383)</t>
+  </si>
+  <si>
+    <t>(-0.14, -0.111)</t>
+  </si>
+  <si>
+    <t>(-0.247, -0.217)</t>
+  </si>
+  <si>
+    <t>(-0.099, -0.07)</t>
+  </si>
+  <si>
+    <t>(-0.319, -0.292)</t>
+  </si>
+  <si>
+    <t>(-0.021, 0.007)</t>
+  </si>
+  <si>
+    <t>(0.034, 0.058)</t>
+  </si>
+  <si>
+    <t>(0.199, 0.224)</t>
+  </si>
+  <si>
+    <t>(-0.025, -0.001)</t>
+  </si>
+  <si>
+    <t>(0.113, 0.138)</t>
+  </si>
+  <si>
+    <t>(-0.141, -0.116)</t>
+  </si>
+  <si>
+    <t>(0.06, 0.084)</t>
+  </si>
+  <si>
+    <t>(-0.118, -0.099)</t>
+  </si>
+  <si>
+    <t>(0.084, 0.105)</t>
+  </si>
+  <si>
+    <t>(0.018, 0.036)</t>
+  </si>
+  <si>
+    <t>(0.25, 0.269)</t>
+  </si>
+  <si>
+    <t>(-0.158, -0.141)</t>
+  </si>
+  <si>
+    <t>(0.047, 0.065)</t>
+  </si>
+  <si>
+    <t>(0.155, 0.171)</t>
+  </si>
+  <si>
+    <t>(0.06, 0.077)</t>
+  </si>
+  <si>
+    <t>(-0.249, -0.234)</t>
+  </si>
+  <si>
+    <t>(0.03, 0.045)</t>
+  </si>
+  <si>
+    <t>(-0.254, -0.222)</t>
+  </si>
+  <si>
+    <t>(-0.29, -0.256)</t>
+  </si>
+  <si>
+    <t>(-0.189, -0.16)</t>
+  </si>
+  <si>
+    <t>(0.028, 0.058)</t>
+  </si>
+  <si>
+    <t>(-0.34, -0.31)</t>
+  </si>
+  <si>
+    <t>(-0.172, -0.143)</t>
+  </si>
+  <si>
+    <t>(-0.035, -0.01)</t>
+  </si>
+  <si>
+    <t>(0.173, 0.201)</t>
+  </si>
+  <si>
+    <t>(-1.572, -1.554)</t>
+  </si>
+  <si>
+    <t>(-0.584, -0.558)</t>
+  </si>
+  <si>
+    <t>(-0.661, -0.637)</t>
+  </si>
+  <si>
+    <t>(-0.891, -0.854)</t>
+  </si>
+  <si>
+    <t>(-0.938, -0.905)</t>
+  </si>
+  <si>
+    <t>(-0.716, -0.687)</t>
+  </si>
+  <si>
+    <t>(-0.975, -0.941)</t>
+  </si>
+  <si>
+    <t>(-0.898, -0.861)</t>
+  </si>
+  <si>
+    <t>(0.921, 0.937)</t>
+  </si>
+  <si>
+    <t>(0.795, 0.811)</t>
+  </si>
+  <si>
+    <t>(0.572, 0.586)</t>
+  </si>
+  <si>
+    <t>(0.688, 0.701)</t>
+  </si>
+  <si>
+    <t>(0.447, 0.46)</t>
+  </si>
+  <si>
+    <t>(0.729, 0.741)</t>
+  </si>
+  <si>
+    <t>(0.395, 0.406)</t>
+  </si>
+  <si>
+    <t>(0.145, 0.158)</t>
+  </si>
+  <si>
+    <t>(1.724, 1.745)</t>
+  </si>
+  <si>
+    <t>(1.45, 1.474)</t>
+  </si>
+  <si>
+    <t>(1.477, 1.492)</t>
+  </si>
+  <si>
+    <t>(1.598, 1.614)</t>
+  </si>
+  <si>
+    <t>(1.43, 1.444)</t>
+  </si>
+  <si>
+    <t>(1.473, 1.486)</t>
+  </si>
+  <si>
+    <t>(1.504, 1.516)</t>
+  </si>
+  <si>
+    <t>(1.415, 1.429)</t>
+  </si>
+  <si>
+    <t>(1.677, 1.693)</t>
+  </si>
+  <si>
+    <t>(1.639, 1.657)</t>
+  </si>
+  <si>
+    <t>(1.361, 1.375)</t>
+  </si>
+  <si>
+    <t>(1.172, 1.189)</t>
+  </si>
+  <si>
+    <t>(1.197, 1.213)</t>
+  </si>
+  <si>
+    <t>(1.405, 1.42)</t>
+  </si>
+  <si>
+    <t>(1.122, 1.138)</t>
+  </si>
+  <si>
+    <t>(1.087, 1.104)</t>
+  </si>
+  <si>
+    <t>(0.391, 0.407)</t>
+  </si>
+  <si>
+    <t>(0.282, 0.299)</t>
+  </si>
+  <si>
+    <t>(0.208, 0.221)</t>
+  </si>
+  <si>
+    <t>(0.146, 0.161)</t>
+  </si>
+  <si>
+    <t>(0.294, 0.308)</t>
+  </si>
+  <si>
+    <t>(0.416, 0.429)</t>
+  </si>
+  <si>
+    <t>(0.429, 0.441)</t>
+  </si>
+  <si>
+    <t>(0.406, 0.419)</t>
+  </si>
+  <si>
+    <t>(1.32, 1.339)</t>
+  </si>
+  <si>
+    <t>(1.396, 1.414)</t>
+  </si>
+  <si>
+    <t>(1.346, 1.361)</t>
+  </si>
+  <si>
+    <t>(1.488, 1.506)</t>
+  </si>
+  <si>
+    <t>(1.3, 1.316)</t>
+  </si>
+  <si>
+    <t>(1.396, 1.413)</t>
+  </si>
+  <si>
+    <t>(1.124, 1.138)</t>
+  </si>
+  <si>
+    <t>(1.065, 1.079)</t>
   </si>
 </sst>
 </file>
@@ -251,9 +780,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +793,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,13 +828,13 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,18 +1125,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="2">
+      <c r="B1" s="6">
         <v>2020</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6">
         <v>2021</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6">
         <v>2022</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1505,13 +2040,13 @@
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>0.1901057116</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>0.1245786413</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>0.83817508289999998</v>
       </c>
       <c r="F29">
@@ -1522,13 +2057,13 @@
       <c r="B30">
         <v>2</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>0.20064038949999999</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>0.12866403139999999</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>0.95765789379999999</v>
       </c>
       <c r="F30">
@@ -1539,13 +2074,13 @@
       <c r="B31">
         <v>3</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>0.2029414182</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>0.13228007059999999</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>0.99757113750000004</v>
       </c>
       <c r="F31">
@@ -1556,13 +2091,13 @@
       <c r="B32">
         <v>4</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>0.2012305532</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>0.13388997180000001</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>1.0872164814</v>
       </c>
       <c r="F32">
@@ -1573,13 +2108,13 @@
       <c r="B33">
         <v>5</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>0.20199927919999999</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>0.13409681509999999</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>1.0872164814</v>
       </c>
       <c r="F33">
@@ -1590,13 +2125,13 @@
       <c r="B34">
         <v>6</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>0.2046729293</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>0.13269538340000001</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>1.0872164814</v>
       </c>
       <c r="F34">
@@ -1607,13 +2142,13 @@
       <c r="B35">
         <v>7</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>0.2037681268</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>0.13358940010000001</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>1.0872164814</v>
       </c>
       <c r="F35">
@@ -1624,13 +2159,13 @@
       <c r="B36">
         <v>8</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>0.20496410970000001</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>0.13275757839999999</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>1.0872164814</v>
       </c>
       <c r="F36">
@@ -1644,13 +2179,13 @@
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>7.0578047699999993E-2</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <v>4.9135036299999997E-2</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>0.35744459610000001</v>
       </c>
       <c r="F37">
@@ -1661,13 +2196,13 @@
       <c r="B38">
         <v>2</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>7.89229704E-2</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="3">
         <v>5.2576604899999997E-2</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>0.21121726129999999</v>
       </c>
       <c r="F38">
@@ -1678,13 +2213,13 @@
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>8.1963344699999996E-2</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="3">
         <v>5.16641906E-2</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>0.21121726129999999</v>
       </c>
       <c r="F39">
@@ -1695,13 +2230,13 @@
       <c r="B40">
         <v>4</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>8.1621849400000002E-2</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="3">
         <v>5.15050144E-2</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>0.21121726129999999</v>
       </c>
       <c r="F40">
@@ -1712,13 +2247,13 @@
       <c r="B41">
         <v>5</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <v>8.2333335300000005E-2</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>5.1042771399999999E-2</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>0.21121726129999999</v>
       </c>
       <c r="F41">
@@ -1729,13 +2264,13 @@
       <c r="B42">
         <v>6</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <v>8.3052101599999997E-2</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="3">
         <v>5.0326466600000001E-2</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <v>0.21121726129999999</v>
       </c>
       <c r="F42">
@@ -1746,13 +2281,13 @@
       <c r="B43">
         <v>7</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>8.2048893999999997E-2</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="3">
         <v>5.04143752E-2</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="3">
         <v>0.21121726129999999</v>
       </c>
       <c r="F43">
@@ -1763,13 +2298,13 @@
       <c r="B44">
         <v>8</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>8.1723539600000006E-2</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="3">
         <v>4.9808077399999998E-2</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="3">
         <v>0.21121726129999999</v>
       </c>
       <c r="F44">
@@ -1785,8 +2320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58FE35B-40E3-42B8-9716-51C7F560DCC8}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,7 +2361,7 @@
       <c r="B2">
         <v>10358</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.17724768129999999</v>
       </c>
     </row>
@@ -1837,7 +2372,7 @@
       <c r="B3">
         <v>7077</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.1211027071</v>
       </c>
     </row>
@@ -1845,16 +2380,16 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>290.31270747999997</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>740.07746884000005</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>29531</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1865,12 +2400,12 @@
       <c r="B5">
         <v>2732</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>4.6750402099999998E-2</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1879,12 +2414,12 @@
       <c r="B6">
         <v>3656</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>6.2562031599999998E-2</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1893,12 +2428,12 @@
       <c r="B7">
         <v>5170</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>8.8469831299999996E-2</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1907,12 +2442,12 @@
       <c r="B8">
         <v>42677</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.73029535580000005</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1921,12 +2456,12 @@
       <c r="B9">
         <v>1839</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>3.1469249499999997E-2</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1935,27 +2470,27 @@
       <c r="B10">
         <v>20972</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0.35887607379999997</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>1.1906461261000001</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>1.6723132553</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>32.494930785999998</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1963,16 +2498,16 @@
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>3.7078460933000001</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.69971700299999995</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>4.25</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1983,12 +2518,12 @@
       <c r="B13">
         <v>7324</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>0.12532940889999999</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1997,12 +2532,12 @@
       <c r="B14">
         <v>3163</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>5.41257401E-2</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2011,12 +2546,12 @@
       <c r="B15">
         <v>11809</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>0.20207741539999999</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2025,31 +2560,689 @@
       <c r="B16">
         <v>24059</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>0.41170129030000002</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>14.273092850999999</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>135.90821062000001</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>9945</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C84CEA-5CB4-450B-89CA-E8828CA96746}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14" t="s">
+        <v>177</v>
+      </c>
+      <c r="H14" t="s">
+        <v>178</v>
+      </c>
+      <c r="I14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G15" t="s">
+        <v>185</v>
+      </c>
+      <c r="H15" t="s">
+        <v>186</v>
+      </c>
+      <c r="I15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" t="s">
+        <v>191</v>
+      </c>
+      <c r="F16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G16" t="s">
+        <v>193</v>
+      </c>
+      <c r="H16" t="s">
+        <v>194</v>
+      </c>
+      <c r="I16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" t="s">
+        <v>201</v>
+      </c>
+      <c r="H17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" t="s">
+        <v>207</v>
+      </c>
+      <c r="F18" t="s">
+        <v>208</v>
+      </c>
+      <c r="G18" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" t="s">
+        <v>210</v>
+      </c>
+      <c r="I18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19" t="s">
+        <v>215</v>
+      </c>
+      <c r="F19" t="s">
+        <v>216</v>
+      </c>
+      <c r="G19" t="s">
+        <v>217</v>
+      </c>
+      <c r="H19" t="s">
+        <v>218</v>
+      </c>
+      <c r="I19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" t="s">
+        <v>223</v>
+      </c>
+      <c r="F20" t="s">
+        <v>224</v>
+      </c>
+      <c r="G20" t="s">
+        <v>225</v>
+      </c>
+      <c r="H20" t="s">
+        <v>226</v>
+      </c>
+      <c r="I20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" t="s">
+        <v>232</v>
+      </c>
+      <c r="G21" t="s">
+        <v>233</v>
+      </c>
+      <c r="H21" t="s">
+        <v>234</v>
+      </c>
+      <c r="I21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" t="s">
+        <v>238</v>
+      </c>
+      <c r="E22" t="s">
+        <v>239</v>
+      </c>
+      <c r="F22" t="s">
+        <v>240</v>
+      </c>
+      <c r="G22" t="s">
+        <v>241</v>
+      </c>
+      <c r="H22" t="s">
+        <v>242</v>
+      </c>
+      <c r="I22" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First attempt for Fall 2020 results
</commit_message>
<xml_diff>
--- a/Descr.xlsx
+++ b/Descr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FSAN\Adm_Yield\Manuscript\Timing-in-Admission-Yield\Timing-in-Admission-Yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7509FF84-8920-4845-8314-BA005FCBA6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF88FE7-42B3-4AD1-B952-C0BC1DDEC220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7590" yWindow="6540" windowWidth="28800" windowHeight="10755" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="252">
   <si>
     <t>Period</t>
   </si>
@@ -273,505 +273,529 @@
     <t>Period 8</t>
   </si>
   <si>
-    <t>(-7.76, -7.749)</t>
-  </si>
-  <si>
-    <t>(-8.969, -8.957)</t>
-  </si>
-  <si>
-    <t>(-8.001, -7.99)</t>
-  </si>
-  <si>
-    <t>(-7.777, -7.766)</t>
-  </si>
-  <si>
-    <t>(-7.305, -7.295)</t>
-  </si>
-  <si>
-    <t>(-7.7, -7.688)</t>
-  </si>
-  <si>
-    <t>(-6.593, -6.583)</t>
-  </si>
-  <si>
-    <t>(-6.071, -6.06)</t>
-  </si>
-  <si>
-    <t>(0.236, 0.259)</t>
-  </si>
-  <si>
-    <t>(1.095, 1.123)</t>
-  </si>
-  <si>
-    <t>(0.888, 0.916)</t>
-  </si>
-  <si>
-    <t>(1.212, 1.248)</t>
-  </si>
-  <si>
-    <t>(1.037, 1.072)</t>
-  </si>
-  <si>
-    <t>(1.333, 1.368)</t>
-  </si>
-  <si>
-    <t>(1.799, 1.822)</t>
-  </si>
-  <si>
-    <t>(1.081, 1.118)</t>
-  </si>
-  <si>
-    <t>(-0.086, -0.074)</t>
-  </si>
-  <si>
-    <t>(-0.346, -0.326)</t>
-  </si>
-  <si>
-    <t>(-0.057, -0.047)</t>
-  </si>
-  <si>
-    <t>(0.025, 0.034)</t>
-  </si>
-  <si>
-    <t>(-0.196, -0.182)</t>
-  </si>
-  <si>
-    <t>(-0.035, -0.026)</t>
-  </si>
-  <si>
-    <t>(-0.077, -0.069)</t>
-  </si>
-  <si>
-    <t>(-0.104, -0.095)</t>
-  </si>
-  <si>
-    <t>(-0.19, -0.17)</t>
-  </si>
-  <si>
-    <t>(-0.252, -0.231)</t>
-  </si>
-  <si>
-    <t>(-0.001, 0.015)</t>
-  </si>
-  <si>
-    <t>(0.194, 0.211)</t>
-  </si>
-  <si>
-    <t>(-0.101, -0.082)</t>
-  </si>
-  <si>
-    <t>(-0.164, -0.147)</t>
-  </si>
-  <si>
-    <t>(0.065, 0.079)</t>
-  </si>
-  <si>
-    <t>(0.002, 0.019)</t>
-  </si>
-  <si>
-    <t>(0.843, 0.864)</t>
-  </si>
-  <si>
-    <t>(0.88, 0.902)</t>
-  </si>
-  <si>
-    <t>(1.028, 1.047)</t>
-  </si>
-  <si>
-    <t>(0.974, 0.995)</t>
-  </si>
-  <si>
-    <t>(1.007, 1.028)</t>
-  </si>
-  <si>
-    <t>(1.128, 1.146)</t>
-  </si>
-  <si>
-    <t>(1.025, 1.042)</t>
-  </si>
-  <si>
-    <t>(1.101, 1.12)</t>
-  </si>
-  <si>
-    <t>(-0.356, -0.341)</t>
-  </si>
-  <si>
-    <t>(-0.057, -0.041)</t>
-  </si>
-  <si>
-    <t>(-0.308, -0.294)</t>
-  </si>
-  <si>
-    <t>(-0.202, -0.187)</t>
-  </si>
-  <si>
-    <t>(-0.054, -0.041)</t>
-  </si>
-  <si>
-    <t>(0.214, 0.226)</t>
-  </si>
-  <si>
-    <t>(0.069, 0.079)</t>
-  </si>
-  <si>
-    <t>(0.447, 0.458)</t>
-  </si>
-  <si>
-    <t>(-1.0, -0.965)</t>
-  </si>
-  <si>
-    <t>(-0.948, -0.913)</t>
-  </si>
-  <si>
-    <t>(-0.812, -0.779)</t>
-  </si>
-  <si>
-    <t>(-0.585, -0.552)</t>
-  </si>
-  <si>
-    <t>(-0.814, -0.779)</t>
-  </si>
-  <si>
-    <t>(-0.627, -0.594)</t>
-  </si>
-  <si>
-    <t>(-0.779, -0.748)</t>
-  </si>
-  <si>
-    <t>(-1.443, -1.373)</t>
-  </si>
-  <si>
-    <t>(-1.41, -1.342)</t>
-  </si>
-  <si>
-    <t>(-1.518, -1.449)</t>
-  </si>
-  <si>
-    <t>(-1.393, -1.323)</t>
-  </si>
-  <si>
-    <t>(-1.377, -1.308)</t>
-  </si>
-  <si>
-    <t>(-1.407, -1.339)</t>
-  </si>
-  <si>
-    <t>(-1.426, -1.358)</t>
-  </si>
-  <si>
-    <t>(-1.339, -1.272)</t>
-  </si>
-  <si>
-    <t>(-0.091, -0.084)</t>
-  </si>
-  <si>
-    <t>(-0.023, -0.017)</t>
-  </si>
-  <si>
-    <t>(0.027, 0.03)</t>
-  </si>
-  <si>
-    <t>(-0.046, -0.04)</t>
-  </si>
-  <si>
-    <t>(-0.094, -0.087)</t>
-  </si>
-  <si>
-    <t>(-0.026, -0.021)</t>
-  </si>
-  <si>
-    <t>(-0.063, -0.059)</t>
-  </si>
-  <si>
-    <t>(-0.052, -0.047)</t>
-  </si>
-  <si>
-    <t>(0.03, 0.052)</t>
-  </si>
-  <si>
-    <t>(0.11, 0.134)</t>
-  </si>
-  <si>
-    <t>(0.192, 0.211)</t>
-  </si>
-  <si>
-    <t>(0.05, 0.071)</t>
-  </si>
-  <si>
-    <t>(0.093, 0.112)</t>
-  </si>
-  <si>
-    <t>(0.103, 0.122)</t>
-  </si>
-  <si>
-    <t>(0.118, 0.134)</t>
-  </si>
-  <si>
-    <t>(0.499, 0.515)</t>
-  </si>
-  <si>
-    <t>(-0.486, -0.454)</t>
-  </si>
-  <si>
-    <t>(-0.456, -0.424)</t>
-  </si>
-  <si>
-    <t>(-0.537, -0.507)</t>
-  </si>
-  <si>
-    <t>(-0.315, -0.284)</t>
-  </si>
-  <si>
-    <t>(-0.531, -0.502)</t>
-  </si>
-  <si>
-    <t>(-0.458, -0.429)</t>
-  </si>
-  <si>
-    <t>(-0.572, -0.547)</t>
-  </si>
-  <si>
-    <t>(-0.418, -0.393)</t>
-  </si>
-  <si>
-    <t>(-0.329, -0.298)</t>
-  </si>
-  <si>
-    <t>(-0.342, -0.309)</t>
-  </si>
-  <si>
-    <t>(-0.412, -0.383)</t>
-  </si>
-  <si>
-    <t>(-0.14, -0.111)</t>
-  </si>
-  <si>
-    <t>(-0.247, -0.217)</t>
-  </si>
-  <si>
-    <t>(-0.099, -0.07)</t>
-  </si>
-  <si>
-    <t>(-0.319, -0.292)</t>
-  </si>
-  <si>
-    <t>(-0.021, 0.007)</t>
-  </si>
-  <si>
-    <t>(0.034, 0.058)</t>
-  </si>
-  <si>
-    <t>(0.199, 0.224)</t>
-  </si>
-  <si>
-    <t>(-0.025, -0.001)</t>
-  </si>
-  <si>
-    <t>(0.113, 0.138)</t>
-  </si>
-  <si>
-    <t>(-0.141, -0.116)</t>
-  </si>
-  <si>
-    <t>(0.06, 0.084)</t>
-  </si>
-  <si>
-    <t>(-0.118, -0.099)</t>
-  </si>
-  <si>
-    <t>(0.084, 0.105)</t>
-  </si>
-  <si>
-    <t>(0.018, 0.036)</t>
-  </si>
-  <si>
-    <t>(0.25, 0.269)</t>
-  </si>
-  <si>
-    <t>(-0.158, -0.141)</t>
-  </si>
-  <si>
-    <t>(0.047, 0.065)</t>
-  </si>
-  <si>
-    <t>(0.155, 0.171)</t>
-  </si>
-  <si>
-    <t>(0.06, 0.077)</t>
-  </si>
-  <si>
-    <t>(-0.249, -0.234)</t>
-  </si>
-  <si>
-    <t>(0.03, 0.045)</t>
-  </si>
-  <si>
-    <t>(-0.254, -0.222)</t>
-  </si>
-  <si>
-    <t>(-0.29, -0.256)</t>
-  </si>
-  <si>
-    <t>(-0.189, -0.16)</t>
-  </si>
-  <si>
-    <t>(0.028, 0.058)</t>
-  </si>
-  <si>
-    <t>(-0.34, -0.31)</t>
-  </si>
-  <si>
-    <t>(-0.172, -0.143)</t>
-  </si>
-  <si>
-    <t>(-0.035, -0.01)</t>
-  </si>
-  <si>
-    <t>(0.173, 0.201)</t>
-  </si>
-  <si>
-    <t>(-1.572, -1.554)</t>
-  </si>
-  <si>
-    <t>(-0.584, -0.558)</t>
-  </si>
-  <si>
-    <t>(-0.661, -0.637)</t>
-  </si>
-  <si>
-    <t>(-0.891, -0.854)</t>
-  </si>
-  <si>
-    <t>(-0.938, -0.905)</t>
-  </si>
-  <si>
-    <t>(-0.716, -0.687)</t>
-  </si>
-  <si>
-    <t>(-0.975, -0.941)</t>
-  </si>
-  <si>
-    <t>(-0.898, -0.861)</t>
-  </si>
-  <si>
-    <t>(0.921, 0.937)</t>
-  </si>
-  <si>
-    <t>(0.795, 0.811)</t>
-  </si>
-  <si>
-    <t>(0.572, 0.586)</t>
-  </si>
-  <si>
-    <t>(0.688, 0.701)</t>
-  </si>
-  <si>
-    <t>(0.447, 0.46)</t>
-  </si>
-  <si>
-    <t>(0.729, 0.741)</t>
-  </si>
-  <si>
-    <t>(0.395, 0.406)</t>
-  </si>
-  <si>
-    <t>(0.145, 0.158)</t>
-  </si>
-  <si>
-    <t>(1.724, 1.745)</t>
-  </si>
-  <si>
-    <t>(1.45, 1.474)</t>
-  </si>
-  <si>
-    <t>(1.477, 1.492)</t>
-  </si>
-  <si>
-    <t>(1.598, 1.614)</t>
-  </si>
-  <si>
-    <t>(1.43, 1.444)</t>
-  </si>
-  <si>
-    <t>(1.473, 1.486)</t>
-  </si>
-  <si>
-    <t>(1.504, 1.516)</t>
-  </si>
-  <si>
-    <t>(1.415, 1.429)</t>
-  </si>
-  <si>
-    <t>(1.677, 1.693)</t>
-  </si>
-  <si>
-    <t>(1.639, 1.657)</t>
-  </si>
-  <si>
-    <t>(1.361, 1.375)</t>
-  </si>
-  <si>
-    <t>(1.172, 1.189)</t>
-  </si>
-  <si>
-    <t>(1.197, 1.213)</t>
-  </si>
-  <si>
-    <t>(1.405, 1.42)</t>
-  </si>
-  <si>
-    <t>(1.122, 1.138)</t>
-  </si>
-  <si>
-    <t>(1.087, 1.104)</t>
-  </si>
-  <si>
-    <t>(0.391, 0.407)</t>
-  </si>
-  <si>
-    <t>(0.282, 0.299)</t>
-  </si>
-  <si>
-    <t>(0.208, 0.221)</t>
-  </si>
-  <si>
-    <t>(0.146, 0.161)</t>
-  </si>
-  <si>
-    <t>(0.294, 0.308)</t>
-  </si>
-  <si>
-    <t>(0.416, 0.429)</t>
-  </si>
-  <si>
-    <t>(0.429, 0.441)</t>
-  </si>
-  <si>
-    <t>(0.406, 0.419)</t>
-  </si>
-  <si>
-    <t>(1.32, 1.339)</t>
-  </si>
-  <si>
-    <t>(1.396, 1.414)</t>
-  </si>
-  <si>
-    <t>(1.346, 1.361)</t>
-  </si>
-  <si>
-    <t>(1.488, 1.506)</t>
-  </si>
-  <si>
-    <t>(1.3, 1.316)</t>
-  </si>
-  <si>
-    <t>(1.396, 1.413)</t>
-  </si>
-  <si>
-    <t>(1.124, 1.138)</t>
-  </si>
-  <si>
-    <t>(1.065, 1.079)</t>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Home Distance</t>
+  </si>
+  <si>
+    <t>Honor Program</t>
+  </si>
+  <si>
+    <t>Change Major</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Postcard</t>
+  </si>
+  <si>
+    <t>Early Event</t>
+  </si>
+  <si>
+    <t>Campus Tour</t>
+  </si>
+  <si>
+    <t>Decision Day Event</t>
+  </si>
+  <si>
+    <t>Delay Review</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>(-7.65, -7.47, -7.28)</t>
+  </si>
+  <si>
+    <t>(-8.64, -8.46, -8.29)</t>
+  </si>
+  <si>
+    <t>(-7.73, -7.55, -7.37)</t>
+  </si>
+  <si>
+    <t>(-7.59, -7.42, -7.26)</t>
+  </si>
+  <si>
+    <t>(-7.13, -6.97, -6.79)</t>
+  </si>
+  <si>
+    <t>(-7.42, -7.27, -7.09)</t>
+  </si>
+  <si>
+    <t>(-6.51, -6.33, -6.17)</t>
+  </si>
+  <si>
+    <t>(-6.1, -5.93, -5.74)</t>
+  </si>
+  <si>
+    <t>(-0.47, -0.08, 0.3)</t>
+  </si>
+  <si>
+    <t>(0.2, 0.65, 1.06)</t>
+  </si>
+  <si>
+    <t>(0.15, 0.63, 1.04)</t>
+  </si>
+  <si>
+    <t>(0.28, 0.83, 1.42)</t>
+  </si>
+  <si>
+    <t>(0.12, 0.68, 1.22)</t>
+  </si>
+  <si>
+    <t>(0.38, 0.92, 1.49)</t>
+  </si>
+  <si>
+    <t>(1.08, 1.43, 1.76)</t>
+  </si>
+  <si>
+    <t>(0.2, 0.74, 1.32)</t>
+  </si>
+  <si>
+    <t>(-0.3, -0.08, 0.09)</t>
+  </si>
+  <si>
+    <t>(-0.64, -0.33, -0.04)</t>
+  </si>
+  <si>
+    <t>(-0.24, -0.06, 0.09)</t>
+  </si>
+  <si>
+    <t>(-0.13, 0.02, 0.15)</t>
+  </si>
+  <si>
+    <t>(-0.39, -0.18, -0.0)</t>
+  </si>
+  <si>
+    <t>(-0.2, -0.03, 0.11)</t>
+  </si>
+  <si>
+    <t>(-0.21, -0.08, 0.04)</t>
+  </si>
+  <si>
+    <t>(-0.25, -0.1, 0.03)</t>
+  </si>
+  <si>
+    <t>(-0.33, -0.04, 0.23)</t>
+  </si>
+  <si>
+    <t>(-0.45, -0.12, 0.22)</t>
+  </si>
+  <si>
+    <t>(-0.13, 0.13, 0.39)</t>
+  </si>
+  <si>
+    <t>(0.09, 0.36, 0.61)</t>
+  </si>
+  <si>
+    <t>(-0.21, 0.06, 0.36)</t>
+  </si>
+  <si>
+    <t>(-0.25, 0.0, 0.25)</t>
+  </si>
+  <si>
+    <t>(-0.0, 0.23, 0.46)</t>
+  </si>
+  <si>
+    <t>(-0.1, 0.17, 0.41)</t>
+  </si>
+  <si>
+    <t>(0.66, 0.97, 1.24)</t>
+  </si>
+  <si>
+    <t>(0.57, 0.95, 1.31)</t>
+  </si>
+  <si>
+    <t>(0.76, 1.09, 1.4)</t>
+  </si>
+  <si>
+    <t>(0.7, 1.04, 1.37)</t>
+  </si>
+  <si>
+    <t>(0.74, 1.06, 1.36)</t>
+  </si>
+  <si>
+    <t>(0.87, 1.18, 1.48)</t>
+  </si>
+  <si>
+    <t>(0.8, 1.05, 1.31)</t>
+  </si>
+  <si>
+    <t>(0.77, 1.11, 1.42)</t>
+  </si>
+  <si>
+    <t>(-0.59, -0.34, -0.09)</t>
+  </si>
+  <si>
+    <t>(-0.36, -0.08, 0.2)</t>
+  </si>
+  <si>
+    <t>(-0.58, -0.33, -0.11)</t>
+  </si>
+  <si>
+    <t>(-0.49, -0.23, 0.0)</t>
+  </si>
+  <si>
+    <t>(-0.27, -0.06, 0.15)</t>
+  </si>
+  <si>
+    <t>(0.04, 0.21, 0.4)</t>
+  </si>
+  <si>
+    <t>(-0.12, 0.05, 0.23)</t>
+  </si>
+  <si>
+    <t>(0.24, 0.44, 0.61)</t>
+  </si>
+  <si>
+    <t>(-0.98, -0.44, 0.1)</t>
+  </si>
+  <si>
+    <t>(-1.04, -0.43, 0.13)</t>
+  </si>
+  <si>
+    <t>(-0.81, -0.29, 0.26)</t>
+  </si>
+  <si>
+    <t>(-0.58, -0.03, 0.5)</t>
+  </si>
+  <si>
+    <t>(-0.83, -0.26, 0.28)</t>
+  </si>
+  <si>
+    <t>(-0.52, 0.01, 0.56)</t>
+  </si>
+  <si>
+    <t>(-0.55, -0.07, 0.45)</t>
+  </si>
+  <si>
+    <t>(-0.74, -0.22, 0.3)</t>
+  </si>
+  <si>
+    <t>(0.27, 1.27, 2.22)</t>
+  </si>
+  <si>
+    <t>(0.25, 1.28, 2.27)</t>
+  </si>
+  <si>
+    <t>(0.11, 1.18, 2.19)</t>
+  </si>
+  <si>
+    <t>(0.34, 1.33, 2.32)</t>
+  </si>
+  <si>
+    <t>(0.26, 1.32, 2.31)</t>
+  </si>
+  <si>
+    <t>(0.27, 1.3, 2.28)</t>
+  </si>
+  <si>
+    <t>(0.25, 1.3, 2.23)</t>
+  </si>
+  <si>
+    <t>(0.39, 1.39, 2.41)</t>
+  </si>
+  <si>
+    <t>(-0.2, -0.1, -0.01)</t>
+  </si>
+  <si>
+    <t>(-0.14, -0.04, 0.05)</t>
+  </si>
+  <si>
+    <t>(-0.05, 0.02, 0.08)</t>
+  </si>
+  <si>
+    <t>(-0.14, -0.05, 0.03)</t>
+  </si>
+  <si>
+    <t>(-0.12, -0.04, 0.03)</t>
+  </si>
+  <si>
+    <t>(-0.16, -0.08, -0.01)</t>
+  </si>
+  <si>
+    <t>(-0.14, -0.06, 0.0)</t>
+  </si>
+  <si>
+    <t>(-0.26, 0.09, 0.42)</t>
+  </si>
+  <si>
+    <t>(-0.25, 0.15, 0.52)</t>
+  </si>
+  <si>
+    <t>(-0.09, 0.24, 0.54)</t>
+  </si>
+  <si>
+    <t>(-0.22, 0.11, 0.42)</t>
+  </si>
+  <si>
+    <t>(-0.18, 0.14, 0.45)</t>
+  </si>
+  <si>
+    <t>(-0.14, 0.16, 0.44)</t>
+  </si>
+  <si>
+    <t>(-0.11, 0.16, 0.42)</t>
+  </si>
+  <si>
+    <t>(0.3, 0.56, 0.81)</t>
+  </si>
+  <si>
+    <t>(-0.61, -0.1, 0.36)</t>
+  </si>
+  <si>
+    <t>(-0.62, -0.09, 0.42)</t>
+  </si>
+  <si>
+    <t>(-0.66, -0.18, 0.26)</t>
+  </si>
+  <si>
+    <t>(-0.41, 0.07, 0.54)</t>
+  </si>
+  <si>
+    <t>(-0.61, -0.15, 0.29)</t>
+  </si>
+  <si>
+    <t>(-0.51, -0.06, 0.36)</t>
+  </si>
+  <si>
+    <t>(-0.58, -0.21, 0.15)</t>
+  </si>
+  <si>
+    <t>(-0.5, -0.05, 0.38)</t>
+  </si>
+  <si>
+    <t>(-0.52, 0.01, 0.49)</t>
+  </si>
+  <si>
+    <t>(-0.63, -0.02, 0.49)</t>
+  </si>
+  <si>
+    <t>(-0.57, -0.1, 0.33)</t>
+  </si>
+  <si>
+    <t>(-0.24, 0.2, 0.68)</t>
+  </si>
+  <si>
+    <t>(-0.42, 0.08, 0.54)</t>
+  </si>
+  <si>
+    <t>(-0.2, 0.24, 0.71)</t>
+  </si>
+  <si>
+    <t>(-0.42, 0.0, 0.41)</t>
+  </si>
+  <si>
+    <t>(-0.11, 0.33, 0.73)</t>
+  </si>
+  <si>
+    <t>(-0.08, 0.31, 0.69)</t>
+  </si>
+  <si>
+    <t>(0.08, 0.46, 0.89)</t>
+  </si>
+  <si>
+    <t>(-0.11, 0.23, 0.57)</t>
+  </si>
+  <si>
+    <t>(0.03, 0.42, 0.81)</t>
+  </si>
+  <si>
+    <t>(-0.28, 0.15, 0.53)</t>
+  </si>
+  <si>
+    <t>(0.0, 0.36, 0.71)</t>
+  </si>
+  <si>
+    <t>(-0.19, 0.14, 0.49)</t>
+  </si>
+  <si>
+    <t>(0.03, 0.37, 0.71)</t>
+  </si>
+  <si>
+    <t>(0.02, 0.33, 0.63)</t>
+  </si>
+  <si>
+    <t>(0.22, 0.53, 0.87)</t>
+  </si>
+  <si>
+    <t>(-0.14, 0.11, 0.38)</t>
+  </si>
+  <si>
+    <t>(0.13, 0.4, 0.67)</t>
+  </si>
+  <si>
+    <t>(0.24, 0.49, 0.74)</t>
+  </si>
+  <si>
+    <t>(0.16, 0.4, 0.64)</t>
+  </si>
+  <si>
+    <t>(-0.18, 0.04, 0.27)</t>
+  </si>
+  <si>
+    <t>(0.1, 0.34, 0.58)</t>
+  </si>
+  <si>
+    <t>(-0.48, 0.04, 0.54)</t>
+  </si>
+  <si>
+    <t>(-0.57, -0.0, 0.49)</t>
+  </si>
+  <si>
+    <t>(-0.35, 0.09, 0.56)</t>
+  </si>
+  <si>
+    <t>(-0.18, 0.34, 0.81)</t>
+  </si>
+  <si>
+    <t>(-0.52, -0.03, 0.42)</t>
+  </si>
+  <si>
+    <t>(-0.3, 0.15, 0.57)</t>
+  </si>
+  <si>
+    <t>(-0.13, 0.24, 0.61)</t>
+  </si>
+  <si>
+    <t>(0.04, 0.49, 0.92)</t>
+  </si>
+  <si>
+    <t>(-1.69, -1.41, -1.15)</t>
+  </si>
+  <si>
+    <t>(-1.03, -0.65, -0.29)</t>
+  </si>
+  <si>
+    <t>(-1.02, -0.63, -0.28)</t>
+  </si>
+  <si>
+    <t>(-1.44, -0.85, -0.22)</t>
+  </si>
+  <si>
+    <t>(-1.42, -0.9, -0.36)</t>
+  </si>
+  <si>
+    <t>(-1.14, -0.67, -0.24)</t>
+  </si>
+  <si>
+    <t>(-1.45, -0.92, -0.4)</t>
+  </si>
+  <si>
+    <t>(-1.44, -0.84, -0.25)</t>
+  </si>
+  <si>
+    <t>(0.82, 1.06, 1.29)</t>
+  </si>
+  <si>
+    <t>(0.64, 0.91, 1.16)</t>
+  </si>
+  <si>
+    <t>(0.46, 0.66, 0.86)</t>
+  </si>
+  <si>
+    <t>(0.58, 0.8, 1.02)</t>
+  </si>
+  <si>
+    <t>(0.35, 0.55, 0.75)</t>
+  </si>
+  <si>
+    <t>(0.68, 0.86, 1.07)</t>
+  </si>
+  <si>
+    <t>(0.31, 0.5, 0.69)</t>
+  </si>
+  <si>
+    <t>(0.05, 0.26, 0.45)</t>
+  </si>
+  <si>
+    <t>(1.66, 1.98, 2.33)</t>
+  </si>
+  <si>
+    <t>(1.27, 1.66, 2.03)</t>
+  </si>
+  <si>
+    <t>(1.44, 1.7, 1.96)</t>
+  </si>
+  <si>
+    <t>(1.6, 1.83, 2.08)</t>
+  </si>
+  <si>
+    <t>(1.44, 1.67, 1.89)</t>
+  </si>
+  <si>
+    <t>(1.52, 1.75, 1.97)</t>
+  </si>
+  <si>
+    <t>(1.55, 1.75, 1.95)</t>
+  </si>
+  <si>
+    <t>(1.44, 1.66, 1.86)</t>
+  </si>
+  <si>
+    <t>(1.68, 1.92, 2.16)</t>
+  </si>
+  <si>
+    <t>(1.62, 1.89, 2.16)</t>
+  </si>
+  <si>
+    <t>(1.32, 1.57, 1.81)</t>
+  </si>
+  <si>
+    <t>(1.12, 1.39, 1.65)</t>
+  </si>
+  <si>
+    <t>(1.15, 1.42, 1.68)</t>
+  </si>
+  <si>
+    <t>(1.44, 1.66, 1.88)</t>
+  </si>
+  <si>
+    <t>(1.11, 1.35, 1.59)</t>
+  </si>
+  <si>
+    <t>(1.01, 1.31, 1.59)</t>
+  </si>
+  <si>
+    <t>(-0.6, -0.35, -0.1)</t>
+  </si>
+  <si>
+    <t>(-0.54, -0.26, 0.01)</t>
+  </si>
+  <si>
+    <t>(-0.51, -0.28, -0.07)</t>
+  </si>
+  <si>
+    <t>(-0.31, -0.08, 0.17)</t>
+  </si>
+  <si>
+    <t>(-0.36, -0.14, 0.07)</t>
+  </si>
+  <si>
+    <t>(-0.32, -0.1, 0.09)</t>
+  </si>
+  <si>
+    <t>(-0.14, 0.04, 0.22)</t>
+  </si>
+  <si>
+    <t>(-0.09, 0.08, 0.26)</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Time-Varying?</t>
+  </si>
+  <si>
+    <t>Multi-Ethnic</t>
   </si>
 </sst>
 </file>
@@ -1119,10 +1143,13 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" activeCellId="2" sqref="C3:C10 E3:E10 G3:G10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="6">
@@ -2591,16 +2618,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C84CEA-5CB4-450B-89CA-E8828CA96746}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2633,616 +2661,1320 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H10" t="s">
+        <v>159</v>
+      </c>
+      <c r="I10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H11" t="s">
+        <v>167</v>
+      </c>
+      <c r="I11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G12" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" t="s">
+        <v>180</v>
+      </c>
+      <c r="F13" t="s">
+        <v>181</v>
+      </c>
+      <c r="G13" t="s">
+        <v>182</v>
+      </c>
+      <c r="H13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H14" t="s">
+        <v>191</v>
+      </c>
+      <c r="I14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E15" t="s">
+        <v>196</v>
+      </c>
+      <c r="F15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G15" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" t="s">
+        <v>199</v>
+      </c>
+      <c r="I15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E16" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" t="s">
+        <v>205</v>
+      </c>
+      <c r="G16" t="s">
+        <v>206</v>
+      </c>
+      <c r="H16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" t="s">
+        <v>214</v>
+      </c>
+      <c r="H17" t="s">
+        <v>215</v>
+      </c>
+      <c r="I17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" t="s">
+        <v>219</v>
+      </c>
+      <c r="E18" t="s">
+        <v>220</v>
+      </c>
+      <c r="F18" t="s">
+        <v>221</v>
+      </c>
+      <c r="G18" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" t="s">
+        <v>223</v>
+      </c>
+      <c r="I18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D19" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" t="s">
+        <v>229</v>
+      </c>
+      <c r="G19" t="s">
+        <v>230</v>
+      </c>
+      <c r="H19" t="s">
+        <v>231</v>
+      </c>
+      <c r="I19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" t="s">
+        <v>234</v>
+      </c>
+      <c r="D20" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" t="s">
+        <v>236</v>
+      </c>
+      <c r="F20" t="s">
+        <v>237</v>
+      </c>
+      <c r="G20" t="s">
+        <v>238</v>
+      </c>
+      <c r="H20" t="s">
+        <v>239</v>
+      </c>
+      <c r="I20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D21" t="s">
+        <v>243</v>
+      </c>
+      <c r="E21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F21" t="s">
+        <v>245</v>
+      </c>
+      <c r="G21" t="s">
+        <v>246</v>
+      </c>
+      <c r="H21" t="s">
+        <v>247</v>
+      </c>
+      <c r="I21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J24" t="s">
+        <v>249</v>
+      </c>
+      <c r="K24">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" t="s">
+        <v>249</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" t="s">
+        <v>89</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>79</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" t="s">
+        <v>89</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>80</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" t="s">
+        <v>88</v>
+      </c>
+      <c r="J28" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>81</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" t="s">
+        <v>88</v>
+      </c>
+      <c r="J29" t="s">
+        <v>249</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" t="s">
+        <v>89</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" t="s">
+        <v>88</v>
+      </c>
+      <c r="I31" t="s">
+        <v>88</v>
+      </c>
+      <c r="J31" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I32" t="s">
+        <v>88</v>
+      </c>
+      <c r="J32" t="s">
+        <v>89</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" t="s">
+        <v>89</v>
+      </c>
+      <c r="I33" t="s">
+        <v>88</v>
+      </c>
+      <c r="J33" t="s">
+        <v>89</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" t="s">
+        <v>89</v>
+      </c>
+      <c r="H34" t="s">
+        <v>89</v>
+      </c>
+      <c r="I34" t="s">
+        <v>89</v>
+      </c>
+      <c r="J34" t="s">
+        <v>89</v>
+      </c>
+      <c r="K34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>82</v>
       </c>
-      <c r="H2" t="s">
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" t="s">
+        <v>89</v>
+      </c>
+      <c r="I36" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" t="s">
+        <v>89</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" t="s">
+        <v>89</v>
+      </c>
+      <c r="I37" t="s">
+        <v>88</v>
+      </c>
+      <c r="J37" t="s">
+        <v>89</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>251</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38" t="s">
+        <v>88</v>
+      </c>
+      <c r="J38" t="s">
+        <v>89</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>83</v>
       </c>
-      <c r="I2" t="s">
+      <c r="B39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" t="s">
+        <v>88</v>
+      </c>
+      <c r="H39" t="s">
+        <v>88</v>
+      </c>
+      <c r="I39" t="s">
+        <v>88</v>
+      </c>
+      <c r="J39" t="s">
+        <v>249</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" t="s">
+        <v>88</v>
+      </c>
+      <c r="H40" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" t="s">
+        <v>88</v>
+      </c>
+      <c r="J40" t="s">
+        <v>249</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H41" t="s">
+        <v>88</v>
+      </c>
+      <c r="I41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J41" t="s">
+        <v>89</v>
+      </c>
+      <c r="K41">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>86</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" t="s">
+        <v>88</v>
+      </c>
+      <c r="I42" t="s">
+        <v>88</v>
+      </c>
+      <c r="J42" t="s">
+        <v>249</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>87</v>
       </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" t="s">
-        <v>114</v>
-      </c>
-      <c r="H6" t="s">
-        <v>115</v>
-      </c>
-      <c r="I6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" t="s">
-        <v>128</v>
-      </c>
-      <c r="H8" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" t="s">
-        <v>135</v>
-      </c>
-      <c r="F9" t="s">
-        <v>136</v>
-      </c>
-      <c r="G9" t="s">
-        <v>137</v>
-      </c>
-      <c r="H9" t="s">
-        <v>138</v>
-      </c>
-      <c r="I9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>141</v>
-      </c>
-      <c r="D10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G10" t="s">
-        <v>145</v>
-      </c>
-      <c r="H10" t="s">
-        <v>146</v>
-      </c>
-      <c r="I10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F11" t="s">
-        <v>152</v>
-      </c>
-      <c r="G11" t="s">
-        <v>153</v>
-      </c>
-      <c r="H11" t="s">
-        <v>154</v>
-      </c>
-      <c r="I11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" t="s">
-        <v>159</v>
-      </c>
-      <c r="F12" t="s">
-        <v>160</v>
-      </c>
-      <c r="G12" t="s">
-        <v>161</v>
-      </c>
-      <c r="H12" t="s">
-        <v>162</v>
-      </c>
-      <c r="I12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" t="s">
-        <v>167</v>
-      </c>
-      <c r="F13" t="s">
-        <v>168</v>
-      </c>
-      <c r="G13" t="s">
-        <v>169</v>
-      </c>
-      <c r="H13" t="s">
-        <v>170</v>
-      </c>
-      <c r="I13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D14" t="s">
-        <v>174</v>
-      </c>
-      <c r="E14" t="s">
-        <v>175</v>
-      </c>
-      <c r="F14" t="s">
-        <v>176</v>
-      </c>
-      <c r="G14" t="s">
-        <v>177</v>
-      </c>
-      <c r="H14" t="s">
-        <v>178</v>
-      </c>
-      <c r="I14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D15" t="s">
-        <v>182</v>
-      </c>
-      <c r="E15" t="s">
-        <v>183</v>
-      </c>
-      <c r="F15" t="s">
-        <v>184</v>
-      </c>
-      <c r="G15" t="s">
-        <v>185</v>
-      </c>
-      <c r="H15" t="s">
-        <v>186</v>
-      </c>
-      <c r="I15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>188</v>
-      </c>
-      <c r="C16" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16" t="s">
-        <v>190</v>
-      </c>
-      <c r="E16" t="s">
-        <v>191</v>
-      </c>
-      <c r="F16" t="s">
-        <v>192</v>
-      </c>
-      <c r="G16" t="s">
-        <v>193</v>
-      </c>
-      <c r="H16" t="s">
-        <v>194</v>
-      </c>
-      <c r="I16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" t="s">
-        <v>197</v>
-      </c>
-      <c r="D17" t="s">
-        <v>198</v>
-      </c>
-      <c r="E17" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" t="s">
-        <v>200</v>
-      </c>
-      <c r="G17" t="s">
-        <v>201</v>
-      </c>
-      <c r="H17" t="s">
-        <v>202</v>
-      </c>
-      <c r="I17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>204</v>
-      </c>
-      <c r="C18" t="s">
-        <v>205</v>
-      </c>
-      <c r="D18" t="s">
-        <v>206</v>
-      </c>
-      <c r="E18" t="s">
-        <v>207</v>
-      </c>
-      <c r="F18" t="s">
-        <v>208</v>
-      </c>
-      <c r="G18" t="s">
-        <v>209</v>
-      </c>
-      <c r="H18" t="s">
-        <v>210</v>
-      </c>
-      <c r="I18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>212</v>
-      </c>
-      <c r="C19" t="s">
-        <v>213</v>
-      </c>
-      <c r="D19" t="s">
-        <v>214</v>
-      </c>
-      <c r="E19" t="s">
-        <v>215</v>
-      </c>
-      <c r="F19" t="s">
-        <v>216</v>
-      </c>
-      <c r="G19" t="s">
-        <v>217</v>
-      </c>
-      <c r="H19" t="s">
-        <v>218</v>
-      </c>
-      <c r="I19" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>220</v>
-      </c>
-      <c r="C20" t="s">
-        <v>221</v>
-      </c>
-      <c r="D20" t="s">
-        <v>222</v>
-      </c>
-      <c r="E20" t="s">
-        <v>223</v>
-      </c>
-      <c r="F20" t="s">
-        <v>224</v>
-      </c>
-      <c r="G20" t="s">
-        <v>225</v>
-      </c>
-      <c r="H20" t="s">
-        <v>226</v>
-      </c>
-      <c r="I20" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>228</v>
-      </c>
-      <c r="C21" t="s">
-        <v>229</v>
-      </c>
-      <c r="D21" t="s">
-        <v>230</v>
-      </c>
-      <c r="E21" t="s">
-        <v>231</v>
-      </c>
-      <c r="F21" t="s">
-        <v>232</v>
-      </c>
-      <c r="G21" t="s">
-        <v>233</v>
-      </c>
-      <c r="H21" t="s">
-        <v>234</v>
-      </c>
-      <c r="I21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>236</v>
-      </c>
-      <c r="C22" t="s">
-        <v>237</v>
-      </c>
-      <c r="D22" t="s">
-        <v>238</v>
-      </c>
-      <c r="E22" t="s">
-        <v>239</v>
-      </c>
-      <c r="F22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G22" t="s">
-        <v>241</v>
-      </c>
-      <c r="H22" t="s">
-        <v>242</v>
-      </c>
-      <c r="I22" t="s">
-        <v>243</v>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G43" t="s">
+        <v>89</v>
+      </c>
+      <c r="H43" t="s">
+        <v>89</v>
+      </c>
+      <c r="I43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J43" t="s">
+        <v>249</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First attempt for Fall 2021
</commit_message>
<xml_diff>
--- a/Descr.xlsx
+++ b/Descr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FSAN\Adm_Yield\Manuscript\Timing-in-Admission-Yield\Timing-in-Admission-Yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF88FE7-42B3-4AD1-B952-C0BC1DDEC220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18176DC-860F-4B97-A0DA-1FFBD85C9829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Table 3" sheetId="4" r:id="rId3"/>
     <sheet name="Table 4" sheetId="3" r:id="rId4"/>
     <sheet name="Table 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Table 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="413">
   <si>
     <t>Period</t>
   </si>
@@ -796,6 +797,489 @@
   </si>
   <si>
     <t>Multi-Ethnic</t>
+  </si>
+  <si>
+    <t>(-7.9, -7.72, -7.55)</t>
+  </si>
+  <si>
+    <t>(-7.24, -7.05, -6.87)</t>
+  </si>
+  <si>
+    <t>(-7.38, -7.2, -7.03)</t>
+  </si>
+  <si>
+    <t>(-6.55, -6.38, -6.21)</t>
+  </si>
+  <si>
+    <t>(-6.67, -6.49, -6.32)</t>
+  </si>
+  <si>
+    <t>(-6.93, -6.74, -6.57)</t>
+  </si>
+  <si>
+    <t>(-6.88, -6.71, -6.55)</t>
+  </si>
+  <si>
+    <t>(-6.3, -6.12, -5.94)</t>
+  </si>
+  <si>
+    <t>(-0.66, -0.25, 0.14)</t>
+  </si>
+  <si>
+    <t>(-0.81, -0.2, 0.34)</t>
+  </si>
+  <si>
+    <t>(0.25, 0.65, 1.05)</t>
+  </si>
+  <si>
+    <t>(-1.13, -0.4, 0.26)</t>
+  </si>
+  <si>
+    <t>(-0.79, 0.0, 0.78)</t>
+  </si>
+  <si>
+    <t>(-0.77, 0.04, 0.86)</t>
+  </si>
+  <si>
+    <t>(-0.33, 0.4, 1.19)</t>
+  </si>
+  <si>
+    <t>(-0.77, 0.04, 0.85)</t>
+  </si>
+  <si>
+    <t>(-0.36, -0.13, 0.06)</t>
+  </si>
+  <si>
+    <t>(-0.55, -0.24, 0.01)</t>
+  </si>
+  <si>
+    <t>(-0.31, -0.15, -0.01)</t>
+  </si>
+  <si>
+    <t>(-0.11, 0.0, 0.1)</t>
+  </si>
+  <si>
+    <t>(-0.26, -0.12, 0.01)</t>
+  </si>
+  <si>
+    <t>(-0.39, -0.22, -0.07)</t>
+  </si>
+  <si>
+    <t>(-0.27, -0.14, -0.03)</t>
+  </si>
+  <si>
+    <t>(-0.21, -0.08, 0.03)</t>
+  </si>
+  <si>
+    <t>(-1.09, -0.6, -0.18)</t>
+  </si>
+  <si>
+    <t>(-1.15, -0.64, -0.16)</t>
+  </si>
+  <si>
+    <t>(-0.66, -0.27, 0.08)</t>
+  </si>
+  <si>
+    <t>(-0.7, -0.37, -0.06)</t>
+  </si>
+  <si>
+    <t>(-0.56, -0.27, 0.02)</t>
+  </si>
+  <si>
+    <t>(-0.35, -0.08, 0.17)</t>
+  </si>
+  <si>
+    <t>(-0.3, -0.09, 0.12)</t>
+  </si>
+  <si>
+    <t>(-0.24, 0.01, 0.26)</t>
+  </si>
+  <si>
+    <t>(0.7, 1.05, 1.37)</t>
+  </si>
+  <si>
+    <t>(0.03, 0.48, 0.91)</t>
+  </si>
+  <si>
+    <t>(0.18, 0.48, 0.76)</t>
+  </si>
+  <si>
+    <t>(0.35, 0.65, 0.93)</t>
+  </si>
+  <si>
+    <t>(0.46, 0.75, 1.02)</t>
+  </si>
+  <si>
+    <t>(0.53, 0.77, 1.01)</t>
+  </si>
+  <si>
+    <t>(0.33, 0.58, 0.82)</t>
+  </si>
+  <si>
+    <t>(0.53, 0.81, 1.06)</t>
+  </si>
+  <si>
+    <t>(-0.45, -0.13, 0.19)</t>
+  </si>
+  <si>
+    <t>(-0.58, -0.24, 0.06)</t>
+  </si>
+  <si>
+    <t>(-0.48, -0.24, -0.02)</t>
+  </si>
+  <si>
+    <t>(-0.29, -0.06, 0.17)</t>
+  </si>
+  <si>
+    <t>(-0.45, -0.25, -0.06)</t>
+  </si>
+  <si>
+    <t>(-0.28, -0.1, 0.09)</t>
+  </si>
+  <si>
+    <t>(0.07, 0.23, 0.38)</t>
+  </si>
+  <si>
+    <t>(0.15, 0.33, 0.51)</t>
+  </si>
+  <si>
+    <t>(-0.01, 0.7, 1.38)</t>
+  </si>
+  <si>
+    <t>(0.19, 0.89, 1.56)</t>
+  </si>
+  <si>
+    <t>(0.04, 0.69, 1.3)</t>
+  </si>
+  <si>
+    <t>(0.5, 1.15, 1.77)</t>
+  </si>
+  <si>
+    <t>(-0.01, 0.59, 1.21)</t>
+  </si>
+  <si>
+    <t>(0.67, 1.21, 1.79)</t>
+  </si>
+  <si>
+    <t>(0.92, 1.43, 1.95)</t>
+  </si>
+  <si>
+    <t>(0.41, 0.97, 1.49)</t>
+  </si>
+  <si>
+    <t>(3.94, 5.21, 6.69)</t>
+  </si>
+  <si>
+    <t>(3.89, 5.27, 6.65)</t>
+  </si>
+  <si>
+    <t>(3.96, 5.24, 6.49)</t>
+  </si>
+  <si>
+    <t>(4.18, 5.52, 6.88)</t>
+  </si>
+  <si>
+    <t>(3.81, 5.03, 6.35)</t>
+  </si>
+  <si>
+    <t>(3.72, 4.99, 6.28)</t>
+  </si>
+  <si>
+    <t>(3.94, 5.13, 6.47)</t>
+  </si>
+  <si>
+    <t>(3.85, 5.2, 6.5)</t>
+  </si>
+  <si>
+    <t>(-0.16, -0.06, 0.03)</t>
+  </si>
+  <si>
+    <t>(-0.35, -0.19, -0.05)</t>
+  </si>
+  <si>
+    <t>(-0.05, 0.01, 0.07)</t>
+  </si>
+  <si>
+    <t>(-0.16, -0.07, 0.01)</t>
+  </si>
+  <si>
+    <t>(-0.13, -0.05, 0.01)</t>
+  </si>
+  <si>
+    <t>(-0.18, -0.1, -0.02)</t>
+  </si>
+  <si>
+    <t>(-0.06, -0.01, 0.04)</t>
+  </si>
+  <si>
+    <t>(-0.16, -0.08, -0.0)</t>
+  </si>
+  <si>
+    <t>(-0.62, -0.15, 0.28)</t>
+  </si>
+  <si>
+    <t>(-0.88, -0.37, 0.08)</t>
+  </si>
+  <si>
+    <t>(-0.34, 0.01, 0.35)</t>
+  </si>
+  <si>
+    <t>(-0.63, -0.23, 0.12)</t>
+  </si>
+  <si>
+    <t>(-0.41, -0.09, 0.23)</t>
+  </si>
+  <si>
+    <t>(-0.6, -0.28, 0.02)</t>
+  </si>
+  <si>
+    <t>(-0.19, 0.04, 0.29)</t>
+  </si>
+  <si>
+    <t>(0.09, 0.35, 0.6)</t>
+  </si>
+  <si>
+    <t>(-0.75, -0.12, 0.5)</t>
+  </si>
+  <si>
+    <t>(-0.98, -0.38, 0.22)</t>
+  </si>
+  <si>
+    <t>(-1.12, -0.54, -0.04)</t>
+  </si>
+  <si>
+    <t>(-0.65, -0.13, 0.42)</t>
+  </si>
+  <si>
+    <t>(-1.06, -0.53, -0.04)</t>
+  </si>
+  <si>
+    <t>(-0.69, -0.23, 0.19)</t>
+  </si>
+  <si>
+    <t>(-0.64, -0.21, 0.18)</t>
+  </si>
+  <si>
+    <t>(-0.82, -0.36, 0.09)</t>
+  </si>
+  <si>
+    <t>(-0.93, -0.22, 0.48)</t>
+  </si>
+  <si>
+    <t>(-0.6, 0.04, 0.64)</t>
+  </si>
+  <si>
+    <t>(-0.62, -0.07, 0.42)</t>
+  </si>
+  <si>
+    <t>(-0.38, 0.19, 0.76)</t>
+  </si>
+  <si>
+    <t>(-1.2, -0.63, -0.09)</t>
+  </si>
+  <si>
+    <t>(-0.92, -0.42, 0.06)</t>
+  </si>
+  <si>
+    <t>(-0.38, 0.06, 0.42)</t>
+  </si>
+  <si>
+    <t>(-0.51, -0.02, 0.42)</t>
+  </si>
+  <si>
+    <t>(-0.16, 0.33, 0.79)</t>
+  </si>
+  <si>
+    <t>(-0.13, 0.42, 0.91)</t>
+  </si>
+  <si>
+    <t>(-0.1, 0.28, 0.67)</t>
+  </si>
+  <si>
+    <t>(0.11, 0.51, 0.91)</t>
+  </si>
+  <si>
+    <t>(-0.34, 0.07, 0.43)</t>
+  </si>
+  <si>
+    <t>(-0.01, 0.33, 0.65)</t>
+  </si>
+  <si>
+    <t>(0.03, 0.33, 0.65)</t>
+  </si>
+  <si>
+    <t>(-0.13, 0.22, 0.57)</t>
+  </si>
+  <si>
+    <t>(0.24, 0.54, 0.85)</t>
+  </si>
+  <si>
+    <t>(-0.09, 0.27, 0.64)</t>
+  </si>
+  <si>
+    <t>(0.09, 0.38, 0.66)</t>
+  </si>
+  <si>
+    <t>(0.19, 0.48, 0.77)</t>
+  </si>
+  <si>
+    <t>(-0.39, -0.12, 0.13)</t>
+  </si>
+  <si>
+    <t>(-0.26, -0.03, 0.23)</t>
+  </si>
+  <si>
+    <t>(-0.16, 0.05, 0.27)</t>
+  </si>
+  <si>
+    <t>(-0.09, 0.16, 0.43)</t>
+  </si>
+  <si>
+    <t>(-0.58, 0.08, 0.7)</t>
+  </si>
+  <si>
+    <t>(-0.79, -0.08, 0.59)</t>
+  </si>
+  <si>
+    <t>(-0.23, 0.31, 0.8)</t>
+  </si>
+  <si>
+    <t>(-0.58, 0.04, 0.58)</t>
+  </si>
+  <si>
+    <t>(-0.28, 0.16, 0.59)</t>
+  </si>
+  <si>
+    <t>(-0.24, 0.22, 0.64)</t>
+  </si>
+  <si>
+    <t>(-0.86, -0.34, 0.13)</t>
+  </si>
+  <si>
+    <t>(-0.47, 0.07, 0.53)</t>
+  </si>
+  <si>
+    <t>(-2.41, -2.14, -1.86)</t>
+  </si>
+  <si>
+    <t>(-2.27, -1.95, -1.65)</t>
+  </si>
+  <si>
+    <t>(-2.93, -2.62, -2.34)</t>
+  </si>
+  <si>
+    <t>(-2.46, -2.21, -1.96)</t>
+  </si>
+  <si>
+    <t>(-2.34, -1.56, -0.69)</t>
+  </si>
+  <si>
+    <t>(-1.97, -1.34, -0.68)</t>
+  </si>
+  <si>
+    <t>(-1.21, -0.57, -0.0)</t>
+  </si>
+  <si>
+    <t>(-0.72, -0.12, 0.49)</t>
+  </si>
+  <si>
+    <t>(0.18, 0.47, 0.76)</t>
+  </si>
+  <si>
+    <t>(0.15, 0.48, 0.79)</t>
+  </si>
+  <si>
+    <t>(0.29, 0.52, 0.75)</t>
+  </si>
+  <si>
+    <t>(0.3, 0.52, 0.74)</t>
+  </si>
+  <si>
+    <t>(0.01, 0.21, 0.43)</t>
+  </si>
+  <si>
+    <t>(-0.08, 0.09, 0.28)</t>
+  </si>
+  <si>
+    <t>(-0.17, -0.01, 0.15)</t>
+  </si>
+  <si>
+    <t>(-0.51, -0.29, -0.07)</t>
+  </si>
+  <si>
+    <t>(1.21, 1.66, 2.1)</t>
+  </si>
+  <si>
+    <t>(1.36, 1.77, 2.15)</t>
+  </si>
+  <si>
+    <t>(1.27, 1.53, 1.8)</t>
+  </si>
+  <si>
+    <t>(1.4, 1.68, 1.95)</t>
+  </si>
+  <si>
+    <t>(1.14, 1.36, 1.59)</t>
+  </si>
+  <si>
+    <t>(1.14, 1.34, 1.54)</t>
+  </si>
+  <si>
+    <t>(1.18, 1.36, 1.54)</t>
+  </si>
+  <si>
+    <t>(1.5, 1.69, 1.9)</t>
+  </si>
+  <si>
+    <t>(1.04, 1.46, 1.85)</t>
+  </si>
+  <si>
+    <t>(0.61, 1.09, 1.53)</t>
+  </si>
+  <si>
+    <t>(0.86, 1.21, 1.54)</t>
+  </si>
+  <si>
+    <t>(0.4, 0.8, 1.18)</t>
+  </si>
+  <si>
+    <t>(0.62, 0.92, 1.22)</t>
+  </si>
+  <si>
+    <t>(1.26, 1.45, 1.65)</t>
+  </si>
+  <si>
+    <t>(1.39, 1.56, 1.75)</t>
+  </si>
+  <si>
+    <t>(1.07, 1.29, 1.53)</t>
+  </si>
+  <si>
+    <t>(-0.68, -0.38, -0.06)</t>
+  </si>
+  <si>
+    <t>(-0.84, -0.51, -0.21)</t>
+  </si>
+  <si>
+    <t>(-0.34, -0.11, 0.1)</t>
+  </si>
+  <si>
+    <t>(-0.38, -0.12, 0.11)</t>
+  </si>
+  <si>
+    <t>(-0.3, -0.11, 0.07)</t>
+  </si>
+  <si>
+    <t>(-0.1, 0.07, 0.23)</t>
+  </si>
+  <si>
+    <t>(-0.08, 0.06, 0.21)</t>
+  </si>
+  <si>
+    <t>(-0.09, 0.09, 0.25)</t>
+  </si>
+  <si>
+    <t>Important</t>
   </si>
 </sst>
 </file>
@@ -2620,8 +3104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C84CEA-5CB4-450B-89CA-E8828CA96746}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3977,4 +4461,1367 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0E0D99-28EE-485F-ACCB-29F31B008EE5}">
+  <dimension ref="A1:K44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H2" t="s">
+        <v>258</v>
+      </c>
+      <c r="I2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F3" t="s">
+        <v>264</v>
+      </c>
+      <c r="G3" t="s">
+        <v>265</v>
+      </c>
+      <c r="H3" t="s">
+        <v>266</v>
+      </c>
+      <c r="I3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F4" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" t="s">
+        <v>273</v>
+      </c>
+      <c r="H4" t="s">
+        <v>274</v>
+      </c>
+      <c r="I4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" t="s">
+        <v>278</v>
+      </c>
+      <c r="E5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H5" t="s">
+        <v>282</v>
+      </c>
+      <c r="I5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6" t="s">
+        <v>288</v>
+      </c>
+      <c r="G6" t="s">
+        <v>289</v>
+      </c>
+      <c r="H6" t="s">
+        <v>290</v>
+      </c>
+      <c r="I6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F7" t="s">
+        <v>296</v>
+      </c>
+      <c r="G7" t="s">
+        <v>297</v>
+      </c>
+      <c r="H7" t="s">
+        <v>298</v>
+      </c>
+      <c r="I7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>301</v>
+      </c>
+      <c r="D8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F8" t="s">
+        <v>304</v>
+      </c>
+      <c r="G8" t="s">
+        <v>305</v>
+      </c>
+      <c r="H8" t="s">
+        <v>306</v>
+      </c>
+      <c r="I8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C9" t="s">
+        <v>309</v>
+      </c>
+      <c r="D9" t="s">
+        <v>310</v>
+      </c>
+      <c r="E9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F9" t="s">
+        <v>312</v>
+      </c>
+      <c r="G9" t="s">
+        <v>313</v>
+      </c>
+      <c r="H9" t="s">
+        <v>314</v>
+      </c>
+      <c r="I9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>316</v>
+      </c>
+      <c r="C10" t="s">
+        <v>317</v>
+      </c>
+      <c r="D10" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" t="s">
+        <v>319</v>
+      </c>
+      <c r="F10" t="s">
+        <v>320</v>
+      </c>
+      <c r="G10" t="s">
+        <v>321</v>
+      </c>
+      <c r="H10" t="s">
+        <v>322</v>
+      </c>
+      <c r="I10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>324</v>
+      </c>
+      <c r="C11" t="s">
+        <v>325</v>
+      </c>
+      <c r="D11" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" t="s">
+        <v>327</v>
+      </c>
+      <c r="F11" t="s">
+        <v>328</v>
+      </c>
+      <c r="G11" t="s">
+        <v>329</v>
+      </c>
+      <c r="H11" t="s">
+        <v>330</v>
+      </c>
+      <c r="I11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12" t="s">
+        <v>333</v>
+      </c>
+      <c r="D12" t="s">
+        <v>334</v>
+      </c>
+      <c r="E12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F12" t="s">
+        <v>336</v>
+      </c>
+      <c r="G12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H12" t="s">
+        <v>338</v>
+      </c>
+      <c r="I12" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>340</v>
+      </c>
+      <c r="C13" t="s">
+        <v>341</v>
+      </c>
+      <c r="D13" t="s">
+        <v>342</v>
+      </c>
+      <c r="E13" t="s">
+        <v>343</v>
+      </c>
+      <c r="F13" t="s">
+        <v>344</v>
+      </c>
+      <c r="G13" t="s">
+        <v>345</v>
+      </c>
+      <c r="H13" t="s">
+        <v>346</v>
+      </c>
+      <c r="I13" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>348</v>
+      </c>
+      <c r="C14" t="s">
+        <v>349</v>
+      </c>
+      <c r="D14" t="s">
+        <v>350</v>
+      </c>
+      <c r="E14" t="s">
+        <v>351</v>
+      </c>
+      <c r="F14" t="s">
+        <v>352</v>
+      </c>
+      <c r="G14" t="s">
+        <v>353</v>
+      </c>
+      <c r="H14" t="s">
+        <v>354</v>
+      </c>
+      <c r="I14" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>356</v>
+      </c>
+      <c r="C15" t="s">
+        <v>357</v>
+      </c>
+      <c r="D15" t="s">
+        <v>358</v>
+      </c>
+      <c r="E15" t="s">
+        <v>359</v>
+      </c>
+      <c r="F15" t="s">
+        <v>360</v>
+      </c>
+      <c r="G15" t="s">
+        <v>361</v>
+      </c>
+      <c r="H15" t="s">
+        <v>362</v>
+      </c>
+      <c r="I15" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16" t="s">
+        <v>364</v>
+      </c>
+      <c r="C16" t="s">
+        <v>365</v>
+      </c>
+      <c r="D16" t="s">
+        <v>366</v>
+      </c>
+      <c r="E16" t="s">
+        <v>367</v>
+      </c>
+      <c r="F16" t="s">
+        <v>368</v>
+      </c>
+      <c r="G16" t="s">
+        <v>369</v>
+      </c>
+      <c r="H16" t="s">
+        <v>370</v>
+      </c>
+      <c r="I16" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>372</v>
+      </c>
+      <c r="C17" t="s">
+        <v>373</v>
+      </c>
+      <c r="D17" t="s">
+        <v>374</v>
+      </c>
+      <c r="E17" t="s">
+        <v>375</v>
+      </c>
+      <c r="F17" t="s">
+        <v>376</v>
+      </c>
+      <c r="G17" t="s">
+        <v>377</v>
+      </c>
+      <c r="H17" t="s">
+        <v>378</v>
+      </c>
+      <c r="I17" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>380</v>
+      </c>
+      <c r="C18" t="s">
+        <v>381</v>
+      </c>
+      <c r="D18" t="s">
+        <v>382</v>
+      </c>
+      <c r="E18" t="s">
+        <v>383</v>
+      </c>
+      <c r="F18" t="s">
+        <v>384</v>
+      </c>
+      <c r="G18" t="s">
+        <v>385</v>
+      </c>
+      <c r="H18" t="s">
+        <v>386</v>
+      </c>
+      <c r="I18" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>388</v>
+      </c>
+      <c r="C19" t="s">
+        <v>389</v>
+      </c>
+      <c r="D19" t="s">
+        <v>390</v>
+      </c>
+      <c r="E19" t="s">
+        <v>391</v>
+      </c>
+      <c r="F19" t="s">
+        <v>392</v>
+      </c>
+      <c r="G19" t="s">
+        <v>393</v>
+      </c>
+      <c r="H19" t="s">
+        <v>394</v>
+      </c>
+      <c r="I19" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>396</v>
+      </c>
+      <c r="C20" t="s">
+        <v>397</v>
+      </c>
+      <c r="D20" t="s">
+        <v>398</v>
+      </c>
+      <c r="E20" t="s">
+        <v>399</v>
+      </c>
+      <c r="F20" t="s">
+        <v>400</v>
+      </c>
+      <c r="G20" t="s">
+        <v>401</v>
+      </c>
+      <c r="H20" t="s">
+        <v>402</v>
+      </c>
+      <c r="I20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>404</v>
+      </c>
+      <c r="C21" t="s">
+        <v>405</v>
+      </c>
+      <c r="D21" t="s">
+        <v>406</v>
+      </c>
+      <c r="E21" t="s">
+        <v>407</v>
+      </c>
+      <c r="F21" t="s">
+        <v>408</v>
+      </c>
+      <c r="G21" t="s">
+        <v>409</v>
+      </c>
+      <c r="H21" t="s">
+        <v>410</v>
+      </c>
+      <c r="I21" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" t="s">
+        <v>412</v>
+      </c>
+      <c r="K24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" t="s">
+        <v>88</v>
+      </c>
+      <c r="K26" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" t="s">
+        <v>88</v>
+      </c>
+      <c r="K27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" t="s">
+        <v>88</v>
+      </c>
+      <c r="K28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" t="s">
+        <v>88</v>
+      </c>
+      <c r="J29" t="s">
+        <v>88</v>
+      </c>
+      <c r="K29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" t="s">
+        <v>88</v>
+      </c>
+      <c r="J30" t="s">
+        <v>88</v>
+      </c>
+      <c r="K30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" t="s">
+        <v>88</v>
+      </c>
+      <c r="I31" t="s">
+        <v>88</v>
+      </c>
+      <c r="J31" t="s">
+        <v>88</v>
+      </c>
+      <c r="K31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I32" t="s">
+        <v>88</v>
+      </c>
+      <c r="J32" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" t="s">
+        <v>89</v>
+      </c>
+      <c r="I33" t="s">
+        <v>88</v>
+      </c>
+      <c r="J33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" t="s">
+        <v>89</v>
+      </c>
+      <c r="H34" t="s">
+        <v>89</v>
+      </c>
+      <c r="I34" t="s">
+        <v>88</v>
+      </c>
+      <c r="J34" t="s">
+        <v>88</v>
+      </c>
+      <c r="K34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" t="s">
+        <v>88</v>
+      </c>
+      <c r="K35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" t="s">
+        <v>89</v>
+      </c>
+      <c r="H36" t="s">
+        <v>89</v>
+      </c>
+      <c r="I36" t="s">
+        <v>89</v>
+      </c>
+      <c r="J36" t="s">
+        <v>88</v>
+      </c>
+      <c r="K36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37" t="s">
+        <v>88</v>
+      </c>
+      <c r="K37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38" t="s">
+        <v>88</v>
+      </c>
+      <c r="K38" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>251</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" t="s">
+        <v>89</v>
+      </c>
+      <c r="I39" t="s">
+        <v>89</v>
+      </c>
+      <c r="J39" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" t="s">
+        <v>88</v>
+      </c>
+      <c r="H40" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" t="s">
+        <v>89</v>
+      </c>
+      <c r="J40" t="s">
+        <v>88</v>
+      </c>
+      <c r="K40" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" t="s">
+        <v>89</v>
+      </c>
+      <c r="I41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J41" t="s">
+        <v>88</v>
+      </c>
+      <c r="K41" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" t="s">
+        <v>88</v>
+      </c>
+      <c r="I42" t="s">
+        <v>88</v>
+      </c>
+      <c r="J42" t="s">
+        <v>88</v>
+      </c>
+      <c r="K42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H43" t="s">
+        <v>88</v>
+      </c>
+      <c r="I43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J43" t="s">
+        <v>88</v>
+      </c>
+      <c r="K43" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" t="s">
+        <v>89</v>
+      </c>
+      <c r="H44" t="s">
+        <v>89</v>
+      </c>
+      <c r="I44" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44" t="s">
+        <v>88</v>
+      </c>
+      <c r="K44" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First attempt for Fall 2022
</commit_message>
<xml_diff>
--- a/Descr.xlsx
+++ b/Descr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FSAN\Adm_Yield\Manuscript\Timing-in-Admission-Yield\Timing-in-Admission-Yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18176DC-860F-4B97-A0DA-1FFBD85C9829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61D2FC4-8A3B-4FB2-9E46-B57BDA56AADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Table 4" sheetId="3" r:id="rId4"/>
     <sheet name="Table 5" sheetId="5" r:id="rId5"/>
     <sheet name="Table 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Table 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="573">
   <si>
     <t>Period</t>
   </si>
@@ -1280,6 +1281,486 @@
   </si>
   <si>
     <t>Important</t>
+  </si>
+  <si>
+    <t>(-9.01, -8.83, -8.65)</t>
+  </si>
+  <si>
+    <t>(-7.36, -7.17, -6.99)</t>
+  </si>
+  <si>
+    <t>(-7.78, -7.62, -7.44)</t>
+  </si>
+  <si>
+    <t>(-7.34, -7.17, -6.99)</t>
+  </si>
+  <si>
+    <t>(-7.5, -7.33, -7.15)</t>
+  </si>
+  <si>
+    <t>(-7.67, -7.49, -7.33)</t>
+  </si>
+  <si>
+    <t>(-6.59, -6.43, -6.27)</t>
+  </si>
+  <si>
+    <t>(-5.81, -5.64, -5.47)</t>
+  </si>
+  <si>
+    <t>(-0.38, 0.05, 0.48)</t>
+  </si>
+  <si>
+    <t>(-0.26, 0.24, 0.67)</t>
+  </si>
+  <si>
+    <t>(-0.24, 0.26, 0.72)</t>
+  </si>
+  <si>
+    <t>(0.79, 1.26, 1.74)</t>
+  </si>
+  <si>
+    <t>(0.06, 0.66, 1.25)</t>
+  </si>
+  <si>
+    <t>(0.09, 0.74, 1.43)</t>
+  </si>
+  <si>
+    <t>(0.14, 0.73, 1.42)</t>
+  </si>
+  <si>
+    <t>(0.17, 0.84, 1.45)</t>
+  </si>
+  <si>
+    <t>(-0.55, -0.26, -0.03)</t>
+  </si>
+  <si>
+    <t>(-0.7, -0.39, -0.12)</t>
+  </si>
+  <si>
+    <t>(-0.29, -0.12, 0.03)</t>
+  </si>
+  <si>
+    <t>(-0.21, -0.03, 0.1)</t>
+  </si>
+  <si>
+    <t>(-0.44, -0.22, -0.04)</t>
+  </si>
+  <si>
+    <t>(-0.31, -0.13, 0.03)</t>
+  </si>
+  <si>
+    <t>(-0.12, -0.02, 0.06)</t>
+  </si>
+  <si>
+    <t>(-0.22, -0.09, 0.02)</t>
+  </si>
+  <si>
+    <t>(-0.82, -0.43, -0.08)</t>
+  </si>
+  <si>
+    <t>(-0.74, -0.34, 0.01)</t>
+  </si>
+  <si>
+    <t>(-0.54, -0.23, 0.05)</t>
+  </si>
+  <si>
+    <t>(-0.24, 0.06, 0.35)</t>
+  </si>
+  <si>
+    <t>(-0.37, -0.08, 0.19)</t>
+  </si>
+  <si>
+    <t>(-0.28, -0.01, 0.25)</t>
+  </si>
+  <si>
+    <t>(-0.25, -0.06, 0.13)</t>
+  </si>
+  <si>
+    <t>(-0.37, -0.09, 0.16)</t>
+  </si>
+  <si>
+    <t>(0.77, 1.1, 1.42)</t>
+  </si>
+  <si>
+    <t>(0.11, 0.5, 0.9)</t>
+  </si>
+  <si>
+    <t>(0.71, 1.04, 1.36)</t>
+  </si>
+  <si>
+    <t>(0.56, 0.9, 1.26)</t>
+  </si>
+  <si>
+    <t>(0.49, 0.79, 1.06)</t>
+  </si>
+  <si>
+    <t>(0.61, 0.9, 1.19)</t>
+  </si>
+  <si>
+    <t>(0.48, 0.71, 0.93)</t>
+  </si>
+  <si>
+    <t>(0.83, 1.09, 1.32)</t>
+  </si>
+  <si>
+    <t>(-0.68, -0.38, -0.11)</t>
+  </si>
+  <si>
+    <t>(-0.54, -0.24, 0.05)</t>
+  </si>
+  <si>
+    <t>(-0.32, -0.12, 0.09)</t>
+  </si>
+  <si>
+    <t>(-0.3, -0.07, 0.17)</t>
+  </si>
+  <si>
+    <t>(-0.3, -0.1, 0.1)</t>
+  </si>
+  <si>
+    <t>(-0.14, 0.05, 0.24)</t>
+  </si>
+  <si>
+    <t>(-0.17, -0.03, 0.1)</t>
+  </si>
+  <si>
+    <t>(-0.01, 0.16, 0.32)</t>
+  </si>
+  <si>
+    <t>(-0.41, 0.21, 0.8)</t>
+  </si>
+  <si>
+    <t>(-0.56, 0.06, 0.66)</t>
+  </si>
+  <si>
+    <t>(-0.51, 0.04, 0.57)</t>
+  </si>
+  <si>
+    <t>(-0.33, 0.23, 0.79)</t>
+  </si>
+  <si>
+    <t>(-0.39, 0.2, 0.76)</t>
+  </si>
+  <si>
+    <t>(-0.17, 0.41, 0.96)</t>
+  </si>
+  <si>
+    <t>(-0.21, 0.24, 0.69)</t>
+  </si>
+  <si>
+    <t>(-0.39, 0.13, 0.62)</t>
+  </si>
+  <si>
+    <t>(0.97, 2.1, 3.28)</t>
+  </si>
+  <si>
+    <t>(1.09, 2.15, 3.34)</t>
+  </si>
+  <si>
+    <t>(0.94, 2.03, 3.16)</t>
+  </si>
+  <si>
+    <t>(0.98, 2.04, 3.16)</t>
+  </si>
+  <si>
+    <t>(0.76, 1.9, 2.98)</t>
+  </si>
+  <si>
+    <t>(0.96, 2.07, 3.2)</t>
+  </si>
+  <si>
+    <t>(1.09, 2.14, 3.29)</t>
+  </si>
+  <si>
+    <t>(1.02, 2.09, 3.21)</t>
+  </si>
+  <si>
+    <t>(-0.06, 0.02, 0.08)</t>
+  </si>
+  <si>
+    <t>(-0.08, -0.0, 0.07)</t>
+  </si>
+  <si>
+    <t>(-0.09, -0.02, 0.05)</t>
+  </si>
+  <si>
+    <t>(-0.09, -0.02, 0.04)</t>
+  </si>
+  <si>
+    <t>(-0.1, -0.03, 0.04)</t>
+  </si>
+  <si>
+    <t>(-0.1, -0.05, -0.0)</t>
+  </si>
+  <si>
+    <t>(-0.26, -0.17, -0.09)</t>
+  </si>
+  <si>
+    <t>(-0.05, 0.33, 0.71)</t>
+  </si>
+  <si>
+    <t>(-0.24, 0.14, 0.52)</t>
+  </si>
+  <si>
+    <t>(-0.39, -0.04, 0.3)</t>
+  </si>
+  <si>
+    <t>(-0.3, 0.05, 0.38)</t>
+  </si>
+  <si>
+    <t>(0.03, 0.33, 0.63)</t>
+  </si>
+  <si>
+    <t>(-0.11, 0.21, 0.51)</t>
+  </si>
+  <si>
+    <t>(-0.01, 0.2, 0.4)</t>
+  </si>
+  <si>
+    <t>(0.19, 0.41, 0.63)</t>
+  </si>
+  <si>
+    <t>(-0.76, -0.12, 0.41)</t>
+  </si>
+  <si>
+    <t>(-0.49, 0.04, 0.57)</t>
+  </si>
+  <si>
+    <t>(-0.61, -0.12, 0.3)</t>
+  </si>
+  <si>
+    <t>(-0.47, -0.03, 0.41)</t>
+  </si>
+  <si>
+    <t>(-0.29, 0.16, 0.57)</t>
+  </si>
+  <si>
+    <t>(-0.03, 0.38, 0.8)</t>
+  </si>
+  <si>
+    <t>(-0.58, -0.24, 0.08)</t>
+  </si>
+  <si>
+    <t>(-0.5, -0.11, 0.27)</t>
+  </si>
+  <si>
+    <t>(-0.38, 0.22, 0.79)</t>
+  </si>
+  <si>
+    <t>(-0.55, -0.02, 0.49)</t>
+  </si>
+  <si>
+    <t>(-0.74, -0.23, 0.26)</t>
+  </si>
+  <si>
+    <t>(-0.65, -0.12, 0.35)</t>
+  </si>
+  <si>
+    <t>(-0.6, -0.11, 0.35)</t>
+  </si>
+  <si>
+    <t>(-0.24, 0.21, 0.67)</t>
+  </si>
+  <si>
+    <t>(-0.2, 0.16, 0.53)</t>
+  </si>
+  <si>
+    <t>(-0.48, -0.07, 0.3)</t>
+  </si>
+  <si>
+    <t>(0.03, 0.47, 0.92)</t>
+  </si>
+  <si>
+    <t>(-0.07, 0.35, 0.75)</t>
+  </si>
+  <si>
+    <t>(-0.28, 0.11, 0.51)</t>
+  </si>
+  <si>
+    <t>(-0.06, 0.31, 0.69)</t>
+  </si>
+  <si>
+    <t>(-0.09, 0.28, 0.66)</t>
+  </si>
+  <si>
+    <t>(0.14, 0.49, 0.83)</t>
+  </si>
+  <si>
+    <t>(-0.12, 0.16, 0.42)</t>
+  </si>
+  <si>
+    <t>(-0.06, 0.24, 0.55)</t>
+  </si>
+  <si>
+    <t>(0.46, 0.78, 1.12)</t>
+  </si>
+  <si>
+    <t>(0.08, 0.38, 0.66)</t>
+  </si>
+  <si>
+    <t>(-0.17, 0.09, 0.35)</t>
+  </si>
+  <si>
+    <t>(-0.19, 0.08, 0.35)</t>
+  </si>
+  <si>
+    <t>(0.14, 0.42, 0.68)</t>
+  </si>
+  <si>
+    <t>(0.17, 0.4, 0.63)</t>
+  </si>
+  <si>
+    <t>(-0.15, 0.05, 0.26)</t>
+  </si>
+  <si>
+    <t>(-0.22, 0.02, 0.25)</t>
+  </si>
+  <si>
+    <t>(-0.66, 0.03, 0.62)</t>
+  </si>
+  <si>
+    <t>(-0.94, -0.25, 0.38)</t>
+  </si>
+  <si>
+    <t>(-0.73, -0.15, 0.38)</t>
+  </si>
+  <si>
+    <t>(-0.95, -0.35, 0.24)</t>
+  </si>
+  <si>
+    <t>(-0.67, -0.07, 0.52)</t>
+  </si>
+  <si>
+    <t>(-0.29, 0.26, 0.77)</t>
+  </si>
+  <si>
+    <t>(-0.51, -0.03, 0.38)</t>
+  </si>
+  <si>
+    <t>(-0.52, -0.04, 0.4)</t>
+  </si>
+  <si>
+    <t>(-1.13, -0.82, -0.52)</t>
+  </si>
+  <si>
+    <t>(-2.04, -1.76, -1.49)</t>
+  </si>
+  <si>
+    <t>(-0.35, -0.11, 0.13)</t>
+  </si>
+  <si>
+    <t>(-1.49, -0.86, -0.26)</t>
+  </si>
+  <si>
+    <t>(-1.32, -0.73, -0.05)</t>
+  </si>
+  <si>
+    <t>(-0.84, -0.37, 0.06)</t>
+  </si>
+  <si>
+    <t>(-1.0, -0.58, -0.18)</t>
+  </si>
+  <si>
+    <t>(-1.39, -0.74, -0.06)</t>
+  </si>
+  <si>
+    <t>(0.81, 1.09, 1.35)</t>
+  </si>
+  <si>
+    <t>(0.58, 0.85, 1.11)</t>
+  </si>
+  <si>
+    <t>(0.56, 0.77, 0.98)</t>
+  </si>
+  <si>
+    <t>(0.67, 0.9, 1.13)</t>
+  </si>
+  <si>
+    <t>(0.35, 0.55, 0.76)</t>
+  </si>
+  <si>
+    <t>(0.52, 0.71, 0.92)</t>
+  </si>
+  <si>
+    <t>(0.27, 0.42, 0.57)</t>
+  </si>
+  <si>
+    <t>(-0.01, 0.18, 0.37)</t>
+  </si>
+  <si>
+    <t>(1.41, 1.72, 2.04)</t>
+  </si>
+  <si>
+    <t>(1.56, 1.88, 2.17)</t>
+  </si>
+  <si>
+    <t>(1.27, 1.51, 1.76)</t>
+  </si>
+  <si>
+    <t>(1.18, 1.44, 1.71)</t>
+  </si>
+  <si>
+    <t>(1.3, 1.52, 1.76)</t>
+  </si>
+  <si>
+    <t>(1.64, 1.84, 2.04)</t>
+  </si>
+  <si>
+    <t>(1.5, 1.65, 1.8)</t>
+  </si>
+  <si>
+    <t>(1.53, 1.72, 1.91)</t>
+  </si>
+  <si>
+    <t>(1.6, 1.89, 2.2)</t>
+  </si>
+  <si>
+    <t>(1.57, 1.88, 2.18)</t>
+  </si>
+  <si>
+    <t>(1.31, 1.56, 1.82)</t>
+  </si>
+  <si>
+    <t>(1.15, 1.47, 1.79)</t>
+  </si>
+  <si>
+    <t>(2.2, 2.4, 2.59)</t>
+  </si>
+  <si>
+    <t>(1.71, 1.92, 2.14)</t>
+  </si>
+  <si>
+    <t>(2.24, 2.38, 2.52)</t>
+  </si>
+  <si>
+    <t>(1.99, 2.16, 2.34)</t>
+  </si>
+  <si>
+    <t>(-0.5, -0.22, 0.05)</t>
+  </si>
+  <si>
+    <t>(-0.3, -0.05, 0.22)</t>
+  </si>
+  <si>
+    <t>(-0.39, -0.17, 0.05)</t>
+  </si>
+  <si>
+    <t>(-0.51, -0.26, -0.01)</t>
+  </si>
+  <si>
+    <t>(-0.45, -0.23, -0.02)</t>
+  </si>
+  <si>
+    <t>(-0.14, 0.07, 0.26)</t>
+  </si>
+  <si>
+    <t>(0.11, 0.24, 0.38)</t>
+  </si>
+  <si>
+    <t>(0.13, 0.28, 0.43)</t>
+  </si>
+  <si>
+    <t>Important?</t>
   </si>
 </sst>
 </file>
@@ -3104,8 +3585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C84CEA-5CB4-450B-89CA-E8828CA96746}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4100,7 +4581,7 @@
         <v>88</v>
       </c>
       <c r="J33" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -4467,8 +4948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0E0D99-28EE-485F-ACCB-29F31B008EE5}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5824,4 +6305,1366 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA230CB-6442-46D0-B6D2-68E60A0BCD0B}">
+  <dimension ref="A1:K44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F2" t="s">
+        <v>417</v>
+      </c>
+      <c r="G2" t="s">
+        <v>418</v>
+      </c>
+      <c r="H2" t="s">
+        <v>419</v>
+      </c>
+      <c r="I2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C3" t="s">
+        <v>422</v>
+      </c>
+      <c r="D3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E3" t="s">
+        <v>424</v>
+      </c>
+      <c r="F3" t="s">
+        <v>425</v>
+      </c>
+      <c r="G3" t="s">
+        <v>426</v>
+      </c>
+      <c r="H3" t="s">
+        <v>427</v>
+      </c>
+      <c r="I3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C4" t="s">
+        <v>430</v>
+      </c>
+      <c r="D4" t="s">
+        <v>431</v>
+      </c>
+      <c r="E4" t="s">
+        <v>432</v>
+      </c>
+      <c r="F4" t="s">
+        <v>433</v>
+      </c>
+      <c r="G4" t="s">
+        <v>434</v>
+      </c>
+      <c r="H4" t="s">
+        <v>435</v>
+      </c>
+      <c r="I4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C5" t="s">
+        <v>438</v>
+      </c>
+      <c r="D5" t="s">
+        <v>439</v>
+      </c>
+      <c r="E5" t="s">
+        <v>440</v>
+      </c>
+      <c r="F5" t="s">
+        <v>441</v>
+      </c>
+      <c r="G5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H5" t="s">
+        <v>443</v>
+      </c>
+      <c r="I5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D6" t="s">
+        <v>447</v>
+      </c>
+      <c r="E6" t="s">
+        <v>448</v>
+      </c>
+      <c r="F6" t="s">
+        <v>449</v>
+      </c>
+      <c r="G6" t="s">
+        <v>450</v>
+      </c>
+      <c r="H6" t="s">
+        <v>451</v>
+      </c>
+      <c r="I6" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>453</v>
+      </c>
+      <c r="C7" t="s">
+        <v>454</v>
+      </c>
+      <c r="D7" t="s">
+        <v>455</v>
+      </c>
+      <c r="E7" t="s">
+        <v>456</v>
+      </c>
+      <c r="F7" t="s">
+        <v>457</v>
+      </c>
+      <c r="G7" t="s">
+        <v>458</v>
+      </c>
+      <c r="H7" t="s">
+        <v>459</v>
+      </c>
+      <c r="I7" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>461</v>
+      </c>
+      <c r="C8" t="s">
+        <v>462</v>
+      </c>
+      <c r="D8" t="s">
+        <v>463</v>
+      </c>
+      <c r="E8" t="s">
+        <v>464</v>
+      </c>
+      <c r="F8" t="s">
+        <v>465</v>
+      </c>
+      <c r="G8" t="s">
+        <v>466</v>
+      </c>
+      <c r="H8" t="s">
+        <v>467</v>
+      </c>
+      <c r="I8" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>469</v>
+      </c>
+      <c r="C9" t="s">
+        <v>470</v>
+      </c>
+      <c r="D9" t="s">
+        <v>471</v>
+      </c>
+      <c r="E9" t="s">
+        <v>472</v>
+      </c>
+      <c r="F9" t="s">
+        <v>473</v>
+      </c>
+      <c r="G9" t="s">
+        <v>474</v>
+      </c>
+      <c r="H9" t="s">
+        <v>475</v>
+      </c>
+      <c r="I9" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>477</v>
+      </c>
+      <c r="C10" t="s">
+        <v>478</v>
+      </c>
+      <c r="D10" t="s">
+        <v>479</v>
+      </c>
+      <c r="E10" t="s">
+        <v>477</v>
+      </c>
+      <c r="F10" t="s">
+        <v>480</v>
+      </c>
+      <c r="G10" t="s">
+        <v>481</v>
+      </c>
+      <c r="H10" t="s">
+        <v>482</v>
+      </c>
+      <c r="I10" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>484</v>
+      </c>
+      <c r="C11" t="s">
+        <v>485</v>
+      </c>
+      <c r="D11" t="s">
+        <v>486</v>
+      </c>
+      <c r="E11" t="s">
+        <v>487</v>
+      </c>
+      <c r="F11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G11" t="s">
+        <v>489</v>
+      </c>
+      <c r="H11" t="s">
+        <v>490</v>
+      </c>
+      <c r="I11" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>492</v>
+      </c>
+      <c r="C12" t="s">
+        <v>493</v>
+      </c>
+      <c r="D12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E12" t="s">
+        <v>495</v>
+      </c>
+      <c r="F12" t="s">
+        <v>496</v>
+      </c>
+      <c r="G12" t="s">
+        <v>497</v>
+      </c>
+      <c r="H12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I12" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>500</v>
+      </c>
+      <c r="C13" t="s">
+        <v>501</v>
+      </c>
+      <c r="D13" t="s">
+        <v>502</v>
+      </c>
+      <c r="E13" t="s">
+        <v>503</v>
+      </c>
+      <c r="F13" t="s">
+        <v>504</v>
+      </c>
+      <c r="G13" t="s">
+        <v>505</v>
+      </c>
+      <c r="H13" t="s">
+        <v>506</v>
+      </c>
+      <c r="I13" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>508</v>
+      </c>
+      <c r="C14" t="s">
+        <v>509</v>
+      </c>
+      <c r="D14" t="s">
+        <v>510</v>
+      </c>
+      <c r="E14" t="s">
+        <v>511</v>
+      </c>
+      <c r="F14" t="s">
+        <v>512</v>
+      </c>
+      <c r="G14" t="s">
+        <v>513</v>
+      </c>
+      <c r="H14" t="s">
+        <v>514</v>
+      </c>
+      <c r="I14" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>516</v>
+      </c>
+      <c r="C15" t="s">
+        <v>517</v>
+      </c>
+      <c r="D15" t="s">
+        <v>518</v>
+      </c>
+      <c r="E15" t="s">
+        <v>519</v>
+      </c>
+      <c r="F15" t="s">
+        <v>520</v>
+      </c>
+      <c r="G15" t="s">
+        <v>521</v>
+      </c>
+      <c r="H15" t="s">
+        <v>522</v>
+      </c>
+      <c r="I15" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16" t="s">
+        <v>524</v>
+      </c>
+      <c r="C16" t="s">
+        <v>525</v>
+      </c>
+      <c r="D16" t="s">
+        <v>526</v>
+      </c>
+      <c r="E16" t="s">
+        <v>527</v>
+      </c>
+      <c r="F16" t="s">
+        <v>528</v>
+      </c>
+      <c r="G16" t="s">
+        <v>529</v>
+      </c>
+      <c r="H16" t="s">
+        <v>530</v>
+      </c>
+      <c r="I16" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>532</v>
+      </c>
+      <c r="C17" t="s">
+        <v>533</v>
+      </c>
+      <c r="D17" t="s">
+        <v>534</v>
+      </c>
+      <c r="E17" t="s">
+        <v>535</v>
+      </c>
+      <c r="F17" t="s">
+        <v>536</v>
+      </c>
+      <c r="G17" t="s">
+        <v>537</v>
+      </c>
+      <c r="H17" t="s">
+        <v>538</v>
+      </c>
+      <c r="I17" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>540</v>
+      </c>
+      <c r="C18" t="s">
+        <v>541</v>
+      </c>
+      <c r="D18" t="s">
+        <v>542</v>
+      </c>
+      <c r="E18" t="s">
+        <v>543</v>
+      </c>
+      <c r="F18" t="s">
+        <v>544</v>
+      </c>
+      <c r="G18" t="s">
+        <v>545</v>
+      </c>
+      <c r="H18" t="s">
+        <v>546</v>
+      </c>
+      <c r="I18" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>548</v>
+      </c>
+      <c r="C19" t="s">
+        <v>549</v>
+      </c>
+      <c r="D19" t="s">
+        <v>550</v>
+      </c>
+      <c r="E19" t="s">
+        <v>551</v>
+      </c>
+      <c r="F19" t="s">
+        <v>552</v>
+      </c>
+      <c r="G19" t="s">
+        <v>553</v>
+      </c>
+      <c r="H19" t="s">
+        <v>554</v>
+      </c>
+      <c r="I19" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>556</v>
+      </c>
+      <c r="C20" t="s">
+        <v>557</v>
+      </c>
+      <c r="D20" t="s">
+        <v>558</v>
+      </c>
+      <c r="E20" t="s">
+        <v>559</v>
+      </c>
+      <c r="F20" t="s">
+        <v>560</v>
+      </c>
+      <c r="G20" t="s">
+        <v>561</v>
+      </c>
+      <c r="H20" t="s">
+        <v>562</v>
+      </c>
+      <c r="I20" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>564</v>
+      </c>
+      <c r="C21" t="s">
+        <v>565</v>
+      </c>
+      <c r="D21" t="s">
+        <v>566</v>
+      </c>
+      <c r="E21" t="s">
+        <v>567</v>
+      </c>
+      <c r="F21" t="s">
+        <v>568</v>
+      </c>
+      <c r="G21" t="s">
+        <v>569</v>
+      </c>
+      <c r="H21" t="s">
+        <v>570</v>
+      </c>
+      <c r="I21" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" t="s">
+        <v>572</v>
+      </c>
+      <c r="K24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" t="s">
+        <v>88</v>
+      </c>
+      <c r="J26" t="s">
+        <v>88</v>
+      </c>
+      <c r="K26" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" t="s">
+        <v>88</v>
+      </c>
+      <c r="K27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" t="s">
+        <v>88</v>
+      </c>
+      <c r="K28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" t="s">
+        <v>88</v>
+      </c>
+      <c r="J29" t="s">
+        <v>88</v>
+      </c>
+      <c r="K29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" t="s">
+        <v>88</v>
+      </c>
+      <c r="K30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" t="s">
+        <v>89</v>
+      </c>
+      <c r="J31" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I32" t="s">
+        <v>88</v>
+      </c>
+      <c r="J32" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" t="s">
+        <v>88</v>
+      </c>
+      <c r="I33" t="s">
+        <v>88</v>
+      </c>
+      <c r="J33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" t="s">
+        <v>89</v>
+      </c>
+      <c r="H34" t="s">
+        <v>89</v>
+      </c>
+      <c r="I34" t="s">
+        <v>88</v>
+      </c>
+      <c r="J34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" t="s">
+        <v>89</v>
+      </c>
+      <c r="H36" t="s">
+        <v>89</v>
+      </c>
+      <c r="I36" t="s">
+        <v>89</v>
+      </c>
+      <c r="J36" t="s">
+        <v>89</v>
+      </c>
+      <c r="K36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" t="s">
+        <v>89</v>
+      </c>
+      <c r="I37" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37" t="s">
+        <v>88</v>
+      </c>
+      <c r="K37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38" t="s">
+        <v>88</v>
+      </c>
+      <c r="K38" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>251</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" t="s">
+        <v>89</v>
+      </c>
+      <c r="I39" t="s">
+        <v>89</v>
+      </c>
+      <c r="J39" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" t="s">
+        <v>89</v>
+      </c>
+      <c r="H40" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" t="s">
+        <v>88</v>
+      </c>
+      <c r="J40" t="s">
+        <v>88</v>
+      </c>
+      <c r="K40" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H41" t="s">
+        <v>88</v>
+      </c>
+      <c r="I41" t="s">
+        <v>89</v>
+      </c>
+      <c r="J41" t="s">
+        <v>88</v>
+      </c>
+      <c r="K41" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" t="s">
+        <v>88</v>
+      </c>
+      <c r="I42" t="s">
+        <v>88</v>
+      </c>
+      <c r="J42" t="s">
+        <v>88</v>
+      </c>
+      <c r="K42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H43" t="s">
+        <v>88</v>
+      </c>
+      <c r="I43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J43" t="s">
+        <v>88</v>
+      </c>
+      <c r="K43" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" t="s">
+        <v>89</v>
+      </c>
+      <c r="H44" t="s">
+        <v>88</v>
+      </c>
+      <c r="I44" t="s">
+        <v>88</v>
+      </c>
+      <c r="J44" t="s">
+        <v>88</v>
+      </c>
+      <c r="K44" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finish results and findings
</commit_message>
<xml_diff>
--- a/Descr.xlsx
+++ b/Descr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FSAN\Adm_Yield\Manuscript\Timing-in-Admission-Yield\Timing-in-Admission-Yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AAAADE-B8E2-4EAC-9569-FC98827F3984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AF707F-A09E-45FD-B3BA-3AF4D7824606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Table 5 - 2020" sheetId="5" r:id="rId5"/>
     <sheet name="Table 6 - 2021" sheetId="6" r:id="rId6"/>
     <sheet name="Table 7 - 2022" sheetId="7" r:id="rId7"/>
+    <sheet name="Boxplot" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1615,6 +1616,674 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5706271" cy="3820058"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D4A2F87-F9E6-48A8-A6AA-A1823E11B88F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="5706271" cy="3820058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5725324" cy="3839111"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1D4B08B-E08D-4A17-BB2C-1277DA9C2A78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4191000"/>
+          <a:ext cx="5725324" cy="3839111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5658640" cy="3839111"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D835F451-858B-49A3-8D27-EF07ECE1C7FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8191500"/>
+          <a:ext cx="5658640" cy="3839111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5725324" cy="3839111"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6458EDE1-FEF3-4B4A-B350-6845D8E0CEA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12192000"/>
+          <a:ext cx="5725324" cy="3839111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5706271" cy="3791479"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{515E8F30-64C4-4443-9EDD-45F67BCC3C66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="16192500"/>
+          <a:ext cx="5706271" cy="3791479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5677692" cy="3829584"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6671CAB-21D9-4BD8-B463-D5F3AC78A235}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="20193000"/>
+          <a:ext cx="5677692" cy="3829584"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5725324" cy="3820058"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEE8B56D-39FF-410B-8716-90054BDB36F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="24193500"/>
+          <a:ext cx="5725324" cy="3820058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5696745" cy="3791479"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EC3B1F9-7766-4054-B8E8-3B7B30C77E34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28194000"/>
+          <a:ext cx="5696745" cy="3791479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5744377" cy="3810532"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0703BD0-4C86-46D9-81BA-02BBF68E7CEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="32194500"/>
+          <a:ext cx="5744377" cy="3810532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5706271" cy="3810532"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47A59F91-1294-4C55-9576-2AD672D433E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="36195000"/>
+          <a:ext cx="5706271" cy="3810532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>211</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5696745" cy="3820058"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB19115-79F3-46E5-90F8-1A3FDC635040}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="40195500"/>
+          <a:ext cx="5696745" cy="3820058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5696745" cy="3791479"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D341846-E648-435E-AE50-A2B5DADBC97F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="44196000"/>
+          <a:ext cx="5696745" cy="3791479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>253</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5687219" cy="3829584"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{094D39B9-547B-441B-847D-8BC39912C38F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="48196500"/>
+          <a:ext cx="5687219" cy="3829584"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715798" cy="3801005"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C5D1761-0CBB-480B-A992-C330D7C79D6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="52197000"/>
+          <a:ext cx="5715798" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>295</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5658640" cy="3801005"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3FD144B-BC2F-4934-8F8C-734064E6BDBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="56197500"/>
+          <a:ext cx="5658640" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>316</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5696745" cy="3801005"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9BF5EDE-EE16-45D0-A375-E9C9B36E2ABF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="60198000"/>
+          <a:ext cx="5696745" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>337</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5696745" cy="3801005"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B69C3144-CAF5-4ABF-909A-473718D87269}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="64198500"/>
+          <a:ext cx="5696745" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3361,7 +4030,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4534,8 +5203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0E0D99-28EE-485F-ACCB-29F31B008EE5}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5706,8 +6375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA230CB-6442-46D0-B6D2-68E60A0BCD0B}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6873,4 +7542,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7955836-D32E-4846-9CAA-EADD32ABB585}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update partial Results and Discussion
</commit_message>
<xml_diff>
--- a/Descr.xlsx
+++ b/Descr.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FSAN\Adm_Yield\Manuscript\Timing-in-Admission-Yield\Timing-in-Admission-Yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2210E1B3-0702-49AA-8D29-27ACC2AC722E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2878A4F8-54D6-46B0-819D-55BB06FEE350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table 5 - 2020" sheetId="5" r:id="rId3"/>
-    <sheet name="Table 6 - 2021" sheetId="6" r:id="rId4"/>
-    <sheet name="Table 7 - 2022" sheetId="7" r:id="rId5"/>
+    <sheet name="Table 3 - 2020" sheetId="5" r:id="rId3"/>
+    <sheet name="Table 4 - 2021" sheetId="6" r:id="rId4"/>
+    <sheet name="Table 5 - 2022" sheetId="7" r:id="rId5"/>
     <sheet name="Boxplot" sheetId="8" r:id="rId6"/>
     <sheet name="Table 3_do not use" sheetId="4" r:id="rId7"/>
     <sheet name="Table 4_do not use" sheetId="3" r:id="rId8"/>
@@ -1585,7 +1585,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1643,14 +1643,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2602,7 +2602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -2612,18 +2612,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="6">
+      <c r="B1" s="11">
         <v>2020</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11">
         <v>2021</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11">
         <v>2022</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2833,7 +2833,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>1</v>
       </c>
       <c r="B14" t="s">
@@ -2847,7 +2847,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>2</v>
       </c>
       <c r="B15" t="s">
@@ -2861,7 +2861,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>3</v>
       </c>
       <c r="B16" t="s">
@@ -2875,7 +2875,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>4</v>
       </c>
       <c r="B17" t="s">
@@ -2889,7 +2889,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>5</v>
       </c>
       <c r="B18" t="s">
@@ -2903,7 +2903,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>6</v>
       </c>
       <c r="B19" t="s">
@@ -2917,7 +2917,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>7</v>
       </c>
       <c r="B20" t="s">
@@ -2931,7 +2931,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>8</v>
       </c>
       <c r="B21" t="s">
@@ -2945,7 +2945,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>1</v>
       </c>
       <c r="B23" t="s">
@@ -2959,7 +2959,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>2</v>
       </c>
       <c r="B24" t="s">
@@ -2973,7 +2973,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>3</v>
       </c>
       <c r="B25" t="s">
@@ -2987,7 +2987,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>4</v>
       </c>
       <c r="B26" t="s">
@@ -3001,7 +3001,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="6">
         <v>5</v>
       </c>
       <c r="B27" t="s">
@@ -3015,7 +3015,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>6</v>
       </c>
       <c r="B28" t="s">
@@ -3029,7 +3029,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>7</v>
       </c>
       <c r="B29" t="s">
@@ -3043,7 +3043,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>8</v>
       </c>
       <c r="B30" t="s">
@@ -3057,7 +3057,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>1</v>
       </c>
       <c r="B32" t="s">
@@ -3071,7 +3071,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>2</v>
       </c>
       <c r="B33" t="s">
@@ -3085,7 +3085,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>3</v>
       </c>
       <c r="B34" t="s">
@@ -3099,7 +3099,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>4</v>
       </c>
       <c r="B35" t="s">
@@ -3113,7 +3113,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+      <c r="A36" s="6">
         <v>5</v>
       </c>
       <c r="B36" t="s">
@@ -3127,7 +3127,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="A37" s="6">
         <v>6</v>
       </c>
       <c r="B37" t="s">
@@ -3141,7 +3141,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+      <c r="A38" s="6">
         <v>7</v>
       </c>
       <c r="B38" t="s">
@@ -3155,7 +3155,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+      <c r="A39" s="6">
         <v>8</v>
       </c>
       <c r="B39" t="s">
@@ -3225,7 +3225,7 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>8482</v>
       </c>
       <c r="D3" s="2">
@@ -3245,7 +3245,7 @@
       <c r="B5" t="s">
         <v>485</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>0.28599999999999998</v>
       </c>
       <c r="E5">
@@ -3301,10 +3301,10 @@
         <v>486</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>177.58699999999999</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>340.9</v>
       </c>
       <c r="F9" s="4"/>
@@ -3317,7 +3317,7 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>21732</v>
       </c>
       <c r="D10" s="2">
@@ -3334,7 +3334,7 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>2280</v>
       </c>
       <c r="D11" s="2">
@@ -3351,7 +3351,7 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>3457</v>
       </c>
       <c r="D12" s="2">
@@ -3368,7 +3368,7 @@
       <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>5072</v>
       </c>
       <c r="D13" s="2">
@@ -3385,7 +3385,7 @@
       <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>44164</v>
       </c>
       <c r="D14" s="2">
@@ -3402,7 +3402,7 @@
       <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>1813</v>
       </c>
       <c r="D15" s="2">
@@ -3416,7 +3416,7 @@
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="2"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -3429,7 +3429,7 @@
       <c r="B17" t="s">
         <v>487</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>17478</v>
       </c>
       <c r="D17" s="2">
@@ -3446,7 +3446,7 @@
       <c r="B18" t="s">
         <v>491</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>6998</v>
       </c>
       <c r="D18" s="2">
@@ -3463,7 +3463,7 @@
       <c r="B19" t="s">
         <v>488</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>2913</v>
       </c>
       <c r="D19" s="2">
@@ -3480,7 +3480,7 @@
       <c r="B20" t="s">
         <v>489</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>3442.951</v>
       </c>
       <c r="D20" s="2">
@@ -3497,7 +3497,7 @@
       <c r="B21" t="s">
         <v>490</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>3126.7689999999998</v>
       </c>
       <c r="D21" s="2">
@@ -3514,7 +3514,7 @@
       <c r="B22" t="s">
         <v>492</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="10">
         <v>24449</v>
       </c>
       <c r="D22" s="2">
@@ -3522,10 +3522,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="10"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="A32" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3537,7 +3537,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4710,8 +4710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0E0D99-28EE-485F-ACCB-29F31B008EE5}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4779,7 +4779,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>218</v>
       </c>
@@ -5882,8 +5882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA230CB-6442-46D0-B6D2-68E60A0BCD0B}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7055,7 +7055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7955836-D32E-4846-9CAA-EADD32ABB585}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A274" workbookViewId="0">
+    <sheetView topLeftCell="A307" workbookViewId="0">
       <selection activeCell="M261" sqref="M261"/>
     </sheetView>
   </sheetViews>
@@ -7778,8 +7778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58FE35B-40E3-42B8-9716-51C7F560DCC8}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish updating Results and Discussion
</commit_message>
<xml_diff>
--- a/Descr.xlsx
+++ b/Descr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FSAN\Adm_Yield\Manuscript\Timing-in-Admission-Yield\Timing-in-Admission-Yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2878A4F8-54D6-46B0-819D-55BB06FEE350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7E705A-516C-4BF1-B92E-8182DD3A3F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -2602,8 +2602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3537,7 +3537,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4711,7 +4711,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5882,8 +5882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA230CB-6442-46D0-B6D2-68E60A0BCD0B}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7055,8 +7055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7955836-D32E-4846-9CAA-EADD32ABB585}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="M261" sqref="M261"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>